<commit_message>
stuck as a puck
</commit_message>
<xml_diff>
--- a/LIVESTOCK-DATA-ORGANIZATION.xlsx
+++ b/LIVESTOCK-DATA-ORGANIZATION.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="420" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Feed Requ's Data" sheetId="4" r:id="rId1"/>
@@ -11001,7 +11001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -11651,8 +11651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S112"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B84" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="S115" sqref="S115"/>

</xml_diff>

<commit_message>
Finished Field Crops...Now onto Soybean and Canola Meal Calc
</commit_message>
<xml_diff>
--- a/LIVESTOCK-DATA-ORGANIZATION.xlsx
+++ b/LIVESTOCK-DATA-ORGANIZATION.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28740" windowHeight="12660" tabRatio="500" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Feed Requ's Data" sheetId="4" r:id="rId1"/>
@@ -583,9 +583,6 @@
     <t>eggs</t>
   </si>
   <si>
-    <t>chicken</t>
-  </si>
-  <si>
     <t>hogs/pork</t>
   </si>
   <si>
@@ -983,9 +980,6 @@
     <t>result of previous….</t>
   </si>
   <si>
-    <t>turkey</t>
-  </si>
-  <si>
     <t>STATIC</t>
   </si>
   <si>
@@ -1002,6 +996,12 @@
   </si>
   <si>
     <t>chicken/turkey calc?</t>
+  </si>
+  <si>
+    <t>chicken - evicerated weight</t>
+  </si>
+  <si>
+    <t>turkey -  evicerated weight</t>
   </si>
 </sst>
 </file>
@@ -1582,7 +1582,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1854,6 +1854,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3401,19 +3402,19 @@
       <c r="Z5" s="93"/>
     </row>
     <row r="6" spans="2:26" ht="14">
-      <c r="B6" s="212" t="s">
+      <c r="B6" s="213" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="213"/>
-      <c r="D6" s="213"/>
-      <c r="E6" s="213"/>
-      <c r="F6" s="213"/>
-      <c r="G6" s="213"/>
-      <c r="H6" s="213"/>
-      <c r="I6" s="213"/>
-      <c r="J6" s="213"/>
-      <c r="K6" s="213"/>
-      <c r="L6" s="214"/>
+      <c r="C6" s="214"/>
+      <c r="D6" s="214"/>
+      <c r="E6" s="214"/>
+      <c r="F6" s="214"/>
+      <c r="G6" s="214"/>
+      <c r="H6" s="214"/>
+      <c r="I6" s="214"/>
+      <c r="J6" s="214"/>
+      <c r="K6" s="214"/>
+      <c r="L6" s="215"/>
       <c r="M6" s="94"/>
       <c r="U6" s="93"/>
       <c r="V6" s="93"/>
@@ -3524,31 +3525,31 @@
     </row>
     <row r="10" spans="2:26" ht="13" thickBot="1"/>
     <row r="11" spans="2:26" ht="14">
-      <c r="B11" s="212" t="s">
+      <c r="B11" s="213" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="213"/>
-      <c r="D11" s="213"/>
-      <c r="E11" s="213"/>
-      <c r="F11" s="213"/>
-      <c r="G11" s="213"/>
-      <c r="H11" s="213"/>
-      <c r="I11" s="213"/>
-      <c r="J11" s="213"/>
-      <c r="K11" s="213"/>
-      <c r="L11" s="213"/>
-      <c r="M11" s="213"/>
-      <c r="N11" s="213"/>
-      <c r="O11" s="214"/>
-      <c r="P11" s="212" t="s">
+      <c r="C11" s="214"/>
+      <c r="D11" s="214"/>
+      <c r="E11" s="214"/>
+      <c r="F11" s="214"/>
+      <c r="G11" s="214"/>
+      <c r="H11" s="214"/>
+      <c r="I11" s="214"/>
+      <c r="J11" s="214"/>
+      <c r="K11" s="214"/>
+      <c r="L11" s="214"/>
+      <c r="M11" s="214"/>
+      <c r="N11" s="214"/>
+      <c r="O11" s="215"/>
+      <c r="P11" s="213" t="s">
         <v>84</v>
       </c>
-      <c r="Q11" s="213"/>
-      <c r="R11" s="213"/>
-      <c r="S11" s="213"/>
-      <c r="T11" s="213"/>
-      <c r="U11" s="213"/>
-      <c r="V11" s="214"/>
+      <c r="Q11" s="214"/>
+      <c r="R11" s="214"/>
+      <c r="S11" s="214"/>
+      <c r="T11" s="214"/>
+      <c r="U11" s="214"/>
+      <c r="V11" s="215"/>
     </row>
     <row r="12" spans="2:26" ht="14">
       <c r="B12" s="63" t="s">
@@ -4881,19 +4882,19 @@
       <c r="B30" s="31"/>
     </row>
     <row r="31" spans="2:24" s="80" customFormat="1" ht="14">
-      <c r="B31" s="212" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="213"/>
-      <c r="D31" s="213"/>
-      <c r="E31" s="213"/>
-      <c r="F31" s="213"/>
-      <c r="G31" s="213"/>
-      <c r="H31" s="213"/>
-      <c r="I31" s="213"/>
-      <c r="J31" s="213"/>
-      <c r="K31" s="213"/>
-      <c r="L31" s="214"/>
+      <c r="B31" s="213" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="214"/>
+      <c r="D31" s="214"/>
+      <c r="E31" s="214"/>
+      <c r="F31" s="214"/>
+      <c r="G31" s="214"/>
+      <c r="H31" s="214"/>
+      <c r="I31" s="214"/>
+      <c r="J31" s="214"/>
+      <c r="K31" s="214"/>
+      <c r="L31" s="215"/>
       <c r="M31" s="31"/>
       <c r="O31" s="31"/>
       <c r="P31" s="31"/>
@@ -5749,20 +5750,20 @@
       <c r="M50" s="83"/>
     </row>
     <row r="51" spans="2:20" s="80" customFormat="1" ht="14">
-      <c r="B51" s="212" t="s">
+      <c r="B51" s="213" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="213"/>
-      <c r="D51" s="213"/>
-      <c r="E51" s="213"/>
-      <c r="F51" s="213"/>
-      <c r="G51" s="213"/>
-      <c r="H51" s="213"/>
-      <c r="I51" s="213"/>
-      <c r="J51" s="213"/>
-      <c r="K51" s="213"/>
-      <c r="L51" s="213"/>
-      <c r="M51" s="214"/>
+      <c r="C51" s="214"/>
+      <c r="D51" s="214"/>
+      <c r="E51" s="214"/>
+      <c r="F51" s="214"/>
+      <c r="G51" s="214"/>
+      <c r="H51" s="214"/>
+      <c r="I51" s="214"/>
+      <c r="J51" s="214"/>
+      <c r="K51" s="214"/>
+      <c r="L51" s="214"/>
+      <c r="M51" s="215"/>
       <c r="O51" s="31"/>
     </row>
     <row r="52" spans="2:20" s="80" customFormat="1" ht="14">
@@ -6706,13 +6707,13 @@
       <c r="P71" s="34"/>
     </row>
     <row r="72" spans="2:25" ht="14">
-      <c r="B72" s="212" t="s">
+      <c r="B72" s="213" t="s">
         <v>80</v>
       </c>
-      <c r="C72" s="213"/>
-      <c r="D72" s="213"/>
-      <c r="E72" s="213"/>
-      <c r="F72" s="213"/>
+      <c r="C72" s="214"/>
+      <c r="D72" s="214"/>
+      <c r="E72" s="214"/>
+      <c r="F72" s="214"/>
       <c r="G72" s="64"/>
       <c r="K72" s="68"/>
     </row>
@@ -7033,13 +7034,13 @@
       <c r="K82" s="67"/>
     </row>
     <row r="83" spans="2:21" ht="14">
-      <c r="B83" s="212" t="s">
+      <c r="B83" s="213" t="s">
         <v>77</v>
       </c>
-      <c r="C83" s="213"/>
-      <c r="D83" s="213"/>
-      <c r="E83" s="213"/>
-      <c r="F83" s="213"/>
+      <c r="C83" s="214"/>
+      <c r="D83" s="214"/>
+      <c r="E83" s="214"/>
+      <c r="F83" s="214"/>
       <c r="G83" s="66"/>
       <c r="H83" s="66"/>
       <c r="I83" s="65" t="s">
@@ -7346,11 +7347,11 @@
       <c r="P93" s="34"/>
     </row>
     <row r="94" spans="2:21" ht="14">
-      <c r="B94" s="209" t="s">
+      <c r="B94" s="210" t="s">
         <v>69</v>
       </c>
-      <c r="C94" s="210"/>
-      <c r="D94" s="211"/>
+      <c r="C94" s="211"/>
+      <c r="D94" s="212"/>
       <c r="E94" s="42"/>
       <c r="F94" s="34"/>
       <c r="G94" s="41"/>
@@ -7613,7 +7614,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="148" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -7621,7 +7622,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="168" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -7632,7 +7633,7 @@
         <v>60</v>
       </c>
       <c r="B5" s="140" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -7641,7 +7642,7 @@
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="B6" s="140" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -7650,12 +7651,12 @@
         <v>1.8181818181818183</v>
       </c>
       <c r="B7" s="140" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="168" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -7663,20 +7664,20 @@
         <v>60</v>
       </c>
       <c r="B10" s="140" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="140" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B11" s="140" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="168" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -7684,7 +7685,7 @@
         <v>59.92</v>
       </c>
       <c r="B14" s="140" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -7693,7 +7694,7 @@
         <v>1.3599999999999999</v>
       </c>
       <c r="B15" s="140" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -7702,14 +7703,14 @@
         <v>0.59920000000000007</v>
       </c>
       <c r="B16" s="140" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15" thickBot="1"/>
     <row r="18" spans="1:9" ht="15" thickBot="1">
       <c r="A18" s="169"/>
       <c r="F18" s="170" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G18" s="171"/>
     </row>
@@ -7719,7 +7720,7 @@
         <v>2.04</v>
       </c>
       <c r="G19" s="173" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H19" s="173"/>
       <c r="I19" s="174"/>
@@ -7731,7 +7732,7 @@
         <v>1.2223680000000001</v>
       </c>
       <c r="G20" s="176" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H20" s="176"/>
       <c r="I20" s="177"/>
@@ -8517,19 +8518,19 @@
     </row>
     <row r="20" spans="1:14" ht="16" thickBot="1"/>
     <row r="21" spans="1:14">
-      <c r="A21" s="215" t="s">
+      <c r="A21" s="216" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="216"/>
-      <c r="C21" s="216"/>
-      <c r="D21" s="216"/>
-      <c r="E21" s="216"/>
-      <c r="F21" s="216"/>
-      <c r="G21" s="216"/>
-      <c r="H21" s="216"/>
-      <c r="I21" s="216"/>
-      <c r="J21" s="216"/>
-      <c r="K21" s="217"/>
+      <c r="B21" s="217"/>
+      <c r="C21" s="217"/>
+      <c r="D21" s="217"/>
+      <c r="E21" s="217"/>
+      <c r="F21" s="217"/>
+      <c r="G21" s="217"/>
+      <c r="H21" s="217"/>
+      <c r="I21" s="217"/>
+      <c r="J21" s="217"/>
+      <c r="K21" s="218"/>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="20" t="s">
@@ -10051,8 +10052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA55"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10169,7 +10170,7 @@
       </c>
       <c r="D17" s="6"/>
       <c r="Q17" s="139" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
@@ -10188,10 +10189,10 @@
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="Q18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="R18" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="R18" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
@@ -10246,7 +10247,7 @@
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="Q20" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="R20">
         <v>1.8572220638525769</v>
@@ -10285,7 +10286,7 @@
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="Q21" s="138" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R21" s="138">
         <v>2.4762960851367692</v>
@@ -10324,7 +10325,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="Q22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R22">
         <v>3.0953701064209618</v>
@@ -10393,19 +10394,19 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="H25" s="198" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I25" s="15"/>
       <c r="J25" s="181" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="K25" s="15"/>
       <c r="L25" s="181" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="M25" s="15"/>
       <c r="N25" s="182" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="O25" s="15"/>
       <c r="P25" s="197"/>
@@ -10502,7 +10503,7 @@
         <v>129</v>
       </c>
       <c r="L29" s="185" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M29" s="15" t="s">
         <v>128</v>
@@ -10579,13 +10580,13 @@
       <c r="H32" s="196"/>
       <c r="I32" s="15"/>
       <c r="J32" s="184" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
-      <c r="N32" s="186" t="s">
-        <v>137</v>
+      <c r="N32" s="209" t="s">
+        <v>271</v>
       </c>
       <c r="O32" s="15"/>
       <c r="P32" s="197"/>
@@ -10594,13 +10595,13 @@
       <c r="H33" s="196"/>
       <c r="I33" s="15"/>
       <c r="J33" s="186" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
-      <c r="N33" s="186" t="s">
-        <v>266</v>
+      <c r="N33" s="209" t="s">
+        <v>272</v>
       </c>
       <c r="O33" s="15"/>
       <c r="P33" s="197"/>
@@ -10615,7 +10616,7 @@
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
       <c r="N34" s="186" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O34" s="15"/>
       <c r="P34" s="197"/>
@@ -10698,13 +10699,13 @@
       <c r="H39" s="203"/>
       <c r="I39" s="187"/>
       <c r="J39" s="190" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K39" s="187"/>
       <c r="L39" s="187"/>
       <c r="M39" s="187"/>
       <c r="N39" s="191" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="O39" s="187"/>
       <c r="P39" s="204"/>
@@ -10719,7 +10720,7 @@
       <c r="H40" s="203"/>
       <c r="I40" s="187"/>
       <c r="J40" s="192" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="K40" s="187"/>
       <c r="L40" s="187"/>
@@ -10755,7 +10756,7 @@
       <c r="H42" s="203"/>
       <c r="I42" s="187"/>
       <c r="J42" s="191" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="K42" s="187"/>
       <c r="L42" s="187"/>
@@ -11652,10 +11653,10 @@
   <dimension ref="A1:S112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B97" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="S115" sqref="S115"/>
+      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -11679,7 +11680,7 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="153" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B1" s="153"/>
       <c r="C1" s="153"/>
@@ -11687,7 +11688,7 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="154" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" s="154"/>
       <c r="C2" s="154"/>
@@ -11695,92 +11696,92 @@
     </row>
     <row r="3" spans="1:19">
       <c r="A3" s="155" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B3" s="155" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="155"/>
       <c r="D3" s="155"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="B4" s="218" t="s">
+      <c r="B4" s="219" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="219"/>
+      <c r="D4" s="219"/>
+      <c r="E4" s="219"/>
+      <c r="F4" s="219"/>
+      <c r="G4" s="219"/>
+      <c r="H4" s="219"/>
+      <c r="I4" s="219"/>
+      <c r="J4" s="219"/>
+      <c r="K4" s="219"/>
+      <c r="L4" s="219"/>
+      <c r="M4" s="219"/>
+      <c r="N4" s="219"/>
+      <c r="O4" s="219"/>
+      <c r="P4" s="220"/>
+      <c r="Q4" s="221" t="s">
         <v>199</v>
       </c>
-      <c r="C4" s="218"/>
-      <c r="D4" s="218"/>
-      <c r="E4" s="218"/>
-      <c r="F4" s="218"/>
-      <c r="G4" s="218"/>
-      <c r="H4" s="218"/>
-      <c r="I4" s="218"/>
-      <c r="J4" s="218"/>
-      <c r="K4" s="218"/>
-      <c r="L4" s="218"/>
-      <c r="M4" s="218"/>
-      <c r="N4" s="218"/>
-      <c r="O4" s="218"/>
-      <c r="P4" s="219"/>
-      <c r="Q4" s="220" t="s">
-        <v>200</v>
-      </c>
-      <c r="R4" s="221"/>
-      <c r="S4" s="221"/>
+      <c r="R4" s="222"/>
+      <c r="S4" s="222"/>
     </row>
     <row r="5" spans="1:19" s="156" customFormat="1" ht="46.5" customHeight="1">
       <c r="B5" s="156" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="156" t="s">
         <v>201</v>
       </c>
-      <c r="C5" s="156" t="s">
+      <c r="D5" s="156" t="s">
         <v>202</v>
       </c>
-      <c r="D5" s="156" t="s">
+      <c r="E5" s="156" t="s">
         <v>203</v>
       </c>
-      <c r="E5" s="156" t="s">
+      <c r="F5" s="156" t="s">
         <v>204</v>
       </c>
-      <c r="F5" s="156" t="s">
+      <c r="G5" s="156" t="s">
         <v>205</v>
       </c>
-      <c r="G5" s="156" t="s">
+      <c r="H5" s="156" t="s">
         <v>206</v>
       </c>
-      <c r="H5" s="156" t="s">
+      <c r="I5" s="156" t="s">
         <v>207</v>
       </c>
-      <c r="I5" s="156" t="s">
+      <c r="J5" s="156" t="s">
         <v>208</v>
       </c>
-      <c r="J5" s="156" t="s">
+      <c r="K5" s="156" t="s">
         <v>209</v>
       </c>
-      <c r="K5" s="156" t="s">
+      <c r="L5" s="156" t="s">
         <v>210</v>
       </c>
-      <c r="L5" s="156" t="s">
+      <c r="M5" s="156" t="s">
         <v>211</v>
       </c>
-      <c r="M5" s="156" t="s">
+      <c r="N5" s="156" t="s">
         <v>212</v>
       </c>
-      <c r="N5" s="156" t="s">
+      <c r="O5" s="156" t="s">
         <v>213</v>
       </c>
-      <c r="O5" s="156" t="s">
+      <c r="P5" s="156" t="s">
         <v>214</v>
       </c>
-      <c r="P5" s="156" t="s">
+      <c r="Q5" s="157" t="s">
         <v>215</v>
       </c>
-      <c r="Q5" s="157" t="s">
+      <c r="R5" s="158" t="s">
         <v>216</v>
       </c>
-      <c r="R5" s="158" t="s">
+      <c r="S5" s="159" t="s">
         <v>217</v>
-      </c>
-      <c r="S5" s="159" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="6" spans="1:19">
@@ -16867,7 +16868,7 @@
     </row>
     <row r="111" spans="1:19">
       <c r="A111" s="148" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B111" s="160">
         <f>AVERAGE(B98:B107)</f>
@@ -17247,16 +17248,16 @@
         <v>9.3715821862348196</v>
       </c>
       <c r="C22" s="115"/>
-      <c r="D22" s="222" t="s">
+      <c r="D22" s="223" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="223"/>
-      <c r="F22" s="223"/>
-      <c r="G22" s="223"/>
-      <c r="H22" s="223"/>
-      <c r="I22" s="223"/>
-      <c r="J22" s="223"/>
-      <c r="K22" s="223"/>
+      <c r="E22" s="224"/>
+      <c r="F22" s="224"/>
+      <c r="G22" s="224"/>
+      <c r="H22" s="224"/>
+      <c r="I22" s="224"/>
+      <c r="J22" s="224"/>
+      <c r="K22" s="224"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="125" t="s">
@@ -17267,14 +17268,14 @@
         <v>2.916666666666667</v>
       </c>
       <c r="C23" s="119"/>
-      <c r="D23" s="222"/>
-      <c r="E23" s="223"/>
-      <c r="F23" s="223"/>
-      <c r="G23" s="223"/>
-      <c r="H23" s="223"/>
-      <c r="I23" s="223"/>
-      <c r="J23" s="223"/>
-      <c r="K23" s="223"/>
+      <c r="D23" s="223"/>
+      <c r="E23" s="224"/>
+      <c r="F23" s="224"/>
+      <c r="G23" s="224"/>
+      <c r="H23" s="224"/>
+      <c r="I23" s="224"/>
+      <c r="J23" s="224"/>
+      <c r="K23" s="224"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="101" t="s">
@@ -17372,16 +17373,16 @@
         <v>57.243045490211102</v>
       </c>
       <c r="C30" s="119"/>
-      <c r="D30" s="222" t="s">
+      <c r="D30" s="223" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="223"/>
-      <c r="F30" s="223"/>
-      <c r="G30" s="223"/>
-      <c r="H30" s="223"/>
-      <c r="I30" s="223"/>
-      <c r="J30" s="223"/>
-      <c r="K30" s="223"/>
+      <c r="E30" s="224"/>
+      <c r="F30" s="224"/>
+      <c r="G30" s="224"/>
+      <c r="H30" s="224"/>
+      <c r="I30" s="224"/>
+      <c r="J30" s="224"/>
+      <c r="K30" s="224"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="116" t="s">
@@ -17392,14 +17393,14 @@
         <v>0.16371564625850341</v>
       </c>
       <c r="C31" s="119"/>
-      <c r="D31" s="222"/>
-      <c r="E31" s="223"/>
-      <c r="F31" s="223"/>
-      <c r="G31" s="223"/>
-      <c r="H31" s="223"/>
-      <c r="I31" s="223"/>
-      <c r="J31" s="223"/>
-      <c r="K31" s="223"/>
+      <c r="D31" s="223"/>
+      <c r="E31" s="224"/>
+      <c r="F31" s="224"/>
+      <c r="G31" s="224"/>
+      <c r="H31" s="224"/>
+      <c r="I31" s="224"/>
+      <c r="J31" s="224"/>
+      <c r="K31" s="224"/>
     </row>
     <row r="32" spans="1:11">
       <c r="F32">
@@ -17468,7 +17469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -17484,45 +17485,45 @@
   <sheetData>
     <row r="1" spans="1:5" s="148" customFormat="1">
       <c r="A1" s="148" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="152" customFormat="1">
       <c r="A2" s="152" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="152" customFormat="1">
       <c r="A3" s="152" t="s">
-        <v>193</v>
-      </c>
-      <c r="B3" s="224" t="s">
         <v>192</v>
       </c>
-      <c r="C3" s="224"/>
-      <c r="D3" s="224"/>
+      <c r="B3" s="225" t="s">
+        <v>191</v>
+      </c>
+      <c r="C3" s="225"/>
+      <c r="D3" s="225"/>
       <c r="E3" s="152" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="152"/>
       <c r="B4" s="152" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C4" s="152" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D4" s="152" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E4" s="152" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="140" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B5" s="140">
         <v>56</v>
@@ -17534,12 +17535,12 @@
         <v>35</v>
       </c>
       <c r="E5" s="140" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="140" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B6" s="140">
         <v>74</v>
@@ -17551,12 +17552,12 @@
         <v>2</v>
       </c>
       <c r="E6" s="140" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="140" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" s="140">
         <v>70</v>
@@ -17568,12 +17569,12 @@
         <v>1</v>
       </c>
       <c r="E7" s="140" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="140" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B8" s="140">
         <v>75</v>
@@ -17585,12 +17586,12 @@
         <v>0</v>
       </c>
       <c r="E8" s="140" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="140" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="140">
         <v>57</v>
@@ -17602,33 +17603,33 @@
         <v>1</v>
       </c>
       <c r="E9" s="140" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="148" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="152" customFormat="1">
       <c r="A14" s="152" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="152" customFormat="1">
       <c r="A15" s="152" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B15" s="152" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C15" s="152" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="140" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B16" s="140">
         <v>16</v>
@@ -17639,7 +17640,7 @@
     </row>
     <row r="17" spans="1:9">
       <c r="A17" s="151" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B17" s="140">
         <v>12</v>
@@ -17650,7 +17651,7 @@
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="140" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B18" s="140">
         <v>8</v>
@@ -17661,7 +17662,7 @@
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="151" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B19" s="140">
         <v>12</v>
@@ -17672,36 +17673,36 @@
     </row>
     <row r="21" spans="1:9" ht="15">
       <c r="A21" s="148" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="140" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="140" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="140" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="225" t="s">
-        <v>166</v>
-      </c>
-      <c r="B27" s="225"/>
-      <c r="C27" s="225"/>
-      <c r="D27" s="225"/>
-      <c r="E27" s="225"/>
-      <c r="F27" s="225"/>
-      <c r="G27" s="225"/>
-      <c r="H27" s="225"/>
-      <c r="I27" s="225"/>
+      <c r="A27" s="226" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="226"/>
+      <c r="C27" s="226"/>
+      <c r="D27" s="226"/>
+      <c r="E27" s="226"/>
+      <c r="F27" s="226"/>
+      <c r="G27" s="226"/>
+      <c r="H27" s="226"/>
+      <c r="I27" s="226"/>
     </row>
     <row r="28" spans="1:9" s="148" customFormat="1">
       <c r="A28" s="147"/>
@@ -17726,33 +17727,33 @@
     </row>
     <row r="29" spans="1:9" s="148" customFormat="1">
       <c r="A29" s="147" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B29" s="147"/>
       <c r="C29" s="147" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D29" s="147" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E29" s="147" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F29" s="147" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G29" s="147" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H29" s="147"/>
       <c r="I29" s="147"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="146" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B30" s="146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C30" s="145">
         <v>3440</v>
@@ -17766,17 +17767,17 @@
         <v>48160</v>
       </c>
       <c r="G30" s="141" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H30" s="141"/>
       <c r="I30" s="141"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="146" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B31" s="146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C31" s="145">
         <v>15799</v>
@@ -17790,17 +17791,17 @@
         <v>126392</v>
       </c>
       <c r="G31" s="141" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H31" s="141"/>
       <c r="I31" s="141"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="146" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B32" s="146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C32" s="145">
         <v>2713</v>
@@ -17814,17 +17815,17 @@
         <v>37982</v>
       </c>
       <c r="G32" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H32" s="141"/>
       <c r="I32" s="141"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="146" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B33" s="146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C33" s="145">
         <v>4612</v>
@@ -17838,17 +17839,17 @@
         <v>36896</v>
       </c>
       <c r="G33" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H33" s="141"/>
       <c r="I33" s="141"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="146" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B34" s="146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C34" s="141">
         <v>68</v>
@@ -17865,17 +17866,17 @@
         <v>456.96000000000004</v>
       </c>
       <c r="G34" s="141" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H34" s="141"/>
       <c r="I34" s="141"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="146" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B35" s="146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C35" s="141">
         <v>75</v>
@@ -17892,17 +17893,17 @@
         <v>126.00000000000001</v>
       </c>
       <c r="G35" s="141" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H35" s="141"/>
       <c r="I35" s="141"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="146" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B36" s="146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C36" s="145">
         <v>1635</v>
@@ -17919,17 +17920,17 @@
         <v>10987.2</v>
       </c>
       <c r="G36" s="141" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H36" s="141"/>
       <c r="I36" s="141"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="146" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B37" s="146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C37" s="145">
         <v>11603</v>
@@ -17946,17 +17947,17 @@
         <v>19493.04</v>
       </c>
       <c r="G37" s="141" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H37" s="141"/>
       <c r="I37" s="141"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="146" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B38" s="146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C38" s="141">
         <v>89</v>
@@ -17973,17 +17974,17 @@
         <v>598.08000000000004</v>
       </c>
       <c r="G38" s="141" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H38" s="141"/>
       <c r="I38" s="141"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="146" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B39" s="146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C39" s="141">
         <v>284</v>
@@ -18000,7 +18001,7 @@
         <v>477.12000000000006</v>
       </c>
       <c r="G39" s="141" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H39" s="141"/>
       <c r="I39" s="141"/>
@@ -18029,7 +18030,7 @@
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="144" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B41" s="144"/>
       <c r="C41" s="141"/>
@@ -18052,26 +18053,26 @@
     </row>
     <row r="43" spans="1:9" ht="15">
       <c r="B43" s="140" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C43" s="150">
         <f>AVERAGE(D30,D31)</f>
         <v>11</v>
       </c>
       <c r="D43" s="149" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="15">
       <c r="B44" s="140" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C44" s="150">
         <f>AVERAGE(D34,D35)</f>
         <v>4.2</v>
       </c>
       <c r="D44" s="149" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="46" spans="1:9" s="148" customFormat="1">
@@ -18097,33 +18098,33 @@
     </row>
     <row r="47" spans="1:9" s="148" customFormat="1">
       <c r="A47" s="147" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B47" s="147"/>
       <c r="C47" s="147" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D47" s="147" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E47" s="147" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F47" s="147" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G47" s="147" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H47" s="147"/>
       <c r="I47" s="147"/>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" s="146" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B48" s="146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C48" s="145">
         <v>3440</v>
@@ -18137,17 +18138,17 @@
         <v>48160</v>
       </c>
       <c r="G48" s="141" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H48" s="141"/>
       <c r="I48" s="141"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="146" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B49" s="146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C49" s="145">
         <v>2713</v>
@@ -18161,17 +18162,17 @@
         <v>37982</v>
       </c>
       <c r="G49" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H49" s="141"/>
       <c r="I49" s="141"/>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="146" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B50" s="146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C50" s="141">
         <v>68</v>
@@ -18188,17 +18189,17 @@
         <v>456.96000000000004</v>
       </c>
       <c r="G50" s="141" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H50" s="141"/>
       <c r="I50" s="141"/>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="146" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B51" s="146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C51" s="145">
         <v>1635</v>
@@ -18215,17 +18216,17 @@
         <v>10987.2</v>
       </c>
       <c r="G51" s="141" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H51" s="141"/>
       <c r="I51" s="141"/>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="146" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B52" s="146" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C52" s="141">
         <v>89</v>
@@ -18242,7 +18243,7 @@
         <v>598.08000000000004</v>
       </c>
       <c r="G52" s="141" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H52" s="141"/>
       <c r="I52" s="141"/>
@@ -18271,7 +18272,7 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="144" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B54" s="144"/>
       <c r="C54" s="141"/>
@@ -18311,33 +18312,33 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" s="147" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B57" s="147"/>
       <c r="C57" s="147" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D57" s="147" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E57" s="147" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F57" s="147" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G57" s="147" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H57" s="147"/>
       <c r="I57" s="147"/>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" s="146" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B58" s="146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C58" s="145">
         <v>15799</v>
@@ -18351,17 +18352,17 @@
         <v>126392</v>
       </c>
       <c r="G58" s="141" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H58" s="141"/>
       <c r="I58" s="141"/>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" s="146" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B59" s="146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C59" s="145">
         <v>4612</v>
@@ -18375,17 +18376,17 @@
         <v>36896</v>
       </c>
       <c r="G59" s="141" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H59" s="141"/>
       <c r="I59" s="141"/>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" s="146" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B60" s="146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C60" s="141">
         <v>75</v>
@@ -18402,17 +18403,17 @@
         <v>126.00000000000001</v>
       </c>
       <c r="G60" s="141" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H60" s="141"/>
       <c r="I60" s="141"/>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" s="146" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B61" s="146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C61" s="145">
         <v>11603</v>
@@ -18429,17 +18430,17 @@
         <v>19493.04</v>
       </c>
       <c r="G61" s="141" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H61" s="141"/>
       <c r="I61" s="141"/>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" s="146" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B62" s="146" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C62" s="141">
         <v>284</v>
@@ -18456,7 +18457,7 @@
         <v>477.12000000000006</v>
       </c>
       <c r="G62" s="141" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H62" s="141"/>
       <c r="I62" s="141"/>
@@ -18485,7 +18486,7 @@
     </row>
     <row r="64" spans="1:9">
       <c r="A64" s="144" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B64" s="144"/>
       <c r="C64" s="141"/>
@@ -18524,7 +18525,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="3" topLeftCell="RC1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A40" sqref="A40"/>
+      <selection pane="topRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -18537,20 +18538,20 @@
   <sheetData>
     <row r="1" spans="1:507">
       <c r="A1" s="155" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:507">
       <c r="A2" s="155" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:507">
       <c r="A4" s="140" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="140" t="s">
         <v>222</v>
-      </c>
-      <c r="B4" s="140" t="s">
-        <v>223</v>
       </c>
       <c r="C4" s="165">
         <v>26299</v>
@@ -20070,10 +20071,10 @@
     </row>
     <row r="5" spans="1:507">
       <c r="A5" s="140" t="s">
+        <v>223</v>
+      </c>
+      <c r="B5" s="140" t="s">
         <v>224</v>
-      </c>
-      <c r="B5" s="140" t="s">
-        <v>225</v>
       </c>
       <c r="C5" s="140">
         <v>22357</v>
@@ -21593,10 +21594,10 @@
     </row>
     <row r="6" spans="1:507">
       <c r="A6" s="140" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B6" s="140" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C6" s="140">
         <v>8374</v>
@@ -23116,10 +23117,10 @@
     </row>
     <row r="7" spans="1:507">
       <c r="A7" s="140" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B7" s="140" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" s="140">
         <v>12819</v>
@@ -24639,7 +24640,7 @@
     </row>
     <row r="9" spans="1:507">
       <c r="A9" s="140" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:507">
@@ -24647,12 +24648,12 @@
         <v>1</v>
       </c>
       <c r="B10" s="140" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="12" spans="1:507">
       <c r="A12" s="155" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:507">
@@ -26681,10 +26682,10 @@
     </row>
     <row r="15" spans="1:507">
       <c r="A15" s="140" t="s">
+        <v>230</v>
+      </c>
+      <c r="B15" s="140" t="s">
         <v>231</v>
-      </c>
-      <c r="B15" s="140" t="s">
-        <v>232</v>
       </c>
       <c r="C15" s="140">
         <f t="shared" ref="C15:BN15" si="0">C6/C5</f>
@@ -28709,10 +28710,10 @@
     </row>
     <row r="16" spans="1:507">
       <c r="A16" s="140" t="s">
+        <v>232</v>
+      </c>
+      <c r="B16" s="140" t="s">
         <v>233</v>
-      </c>
-      <c r="B16" s="140" t="s">
-        <v>234</v>
       </c>
       <c r="C16" s="140">
         <f t="shared" ref="C16:BN16" si="8">C7/C5</f>
@@ -30741,10 +30742,10 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="148" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B19" s="148" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C19" s="148">
         <f>AVERAGE(RC15:RN15)</f>
@@ -30753,10 +30754,10 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="148" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B20" s="148" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C20" s="148">
         <f>AVERAGE(RC16:RN16)</f>
@@ -30770,10 +30771,10 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="148" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" s="140" t="s">
         <v>236</v>
-      </c>
-      <c r="B22" s="140" t="s">
-        <v>237</v>
       </c>
       <c r="C22" s="166">
         <f>C19*'[2]Field Crops'!C108</f>
@@ -30782,10 +30783,10 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="148" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B23" s="140" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C23" s="166">
         <f>C20*'[2]Field Crops'!C108</f>
@@ -30794,10 +30795,10 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="148" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B25" s="140" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C25" s="166">
         <f>C19*'[2]Field Crops'!C107</f>
@@ -30806,10 +30807,10 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="148" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B26" s="140" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C26" s="166">
         <f>C20*'[2]Field Crops'!C107</f>
@@ -30818,10 +30819,10 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="140" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B28" s="140" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C28" s="167">
         <f>C20*'[2]cansim-0010010-canola CND'!D34</f>
@@ -30843,9 +30844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:SS17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -30856,21 +30855,21 @@
   <sheetData>
     <row r="1" spans="1:513">
       <c r="A1" s="168" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B1" s="168"/>
     </row>
     <row r="2" spans="1:513">
       <c r="A2" s="155" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:513">
       <c r="A4" s="140" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="140" t="s">
         <v>222</v>
-      </c>
-      <c r="B4" s="140" t="s">
-        <v>223</v>
       </c>
       <c r="C4" s="165">
         <v>26146</v>
@@ -32408,10 +32407,10 @@
     </row>
     <row r="5" spans="1:513">
       <c r="A5" s="140" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="140" t="s">
         <v>240</v>
-      </c>
-      <c r="B5" s="140" t="s">
-        <v>241</v>
       </c>
       <c r="C5" s="140">
         <v>54753</v>
@@ -33158,801 +33157,801 @@
         <v>69430</v>
       </c>
       <c r="IQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IT5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IU5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IV5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IW5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IX5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IY5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IZ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JA5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JB5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JC5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JD5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JE5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JF5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JG5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JH5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JI5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JJ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JK5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JL5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JM5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JN5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JO5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JP5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JT5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JU5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JV5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JW5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JX5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JY5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JZ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KA5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KB5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KC5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KD5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KE5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KF5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KG5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KH5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KI5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KJ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KK5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KL5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KM5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KN5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KO5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KP5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KT5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KU5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KV5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KW5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KX5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KY5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KZ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LA5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LB5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LC5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LD5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LE5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LF5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LG5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LH5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LI5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LJ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LK5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LL5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LM5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LN5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LO5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LP5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LT5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LU5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LV5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LW5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LX5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LY5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LZ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MA5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MB5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MC5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MD5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="ME5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MF5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MG5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MH5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MI5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MJ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MK5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="ML5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MM5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MN5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MO5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MP5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MT5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MU5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MV5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MW5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MX5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MY5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MZ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NA5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NB5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NC5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="ND5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NE5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NF5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NG5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NH5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NI5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NJ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NK5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NL5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NM5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NN5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NO5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NP5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NT5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NU5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NV5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NW5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NX5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NY5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NZ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OA5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OB5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OC5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OD5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OE5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OF5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OG5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OH5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OI5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OJ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OK5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OL5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OM5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="ON5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OO5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OP5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OT5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OU5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OV5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OW5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OX5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OY5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OZ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PA5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PB5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PC5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PD5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PE5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PF5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PG5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PH5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PI5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PJ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PK5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PL5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PM5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PN5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PO5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PP5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PT5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PU5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PV5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PW5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PX5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PY5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PZ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QA5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QB5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QC5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QD5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QE5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QF5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QG5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QH5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QI5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QJ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QK5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QL5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QM5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QN5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QO5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QP5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QT5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QU5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QV5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QW5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QX5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QY5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QZ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RA5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RB5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RC5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RD5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RE5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RF5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RG5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RH5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RI5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RJ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RK5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RL5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RM5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RN5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RO5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RP5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RT5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RU5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RV5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RW5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RX5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RY5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RZ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SA5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SB5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SC5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SD5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SE5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SF5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SG5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SH5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SI5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SJ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SK5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SL5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SM5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SN5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SO5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SP5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SQ5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SR5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SS5" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:513">
       <c r="A6" s="140" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B6" s="140" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C6" s="140">
         <v>42758</v>
@@ -34699,798 +34698,798 @@
         <v>53092</v>
       </c>
       <c r="IQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IT6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IU6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IV6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IW6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IX6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IY6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="IZ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JA6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JB6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JC6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JD6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JE6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JF6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JG6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JH6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JI6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JJ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JK6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JL6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JM6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JN6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JO6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JP6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JT6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JU6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JV6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JW6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JX6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JY6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="JZ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KA6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KB6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KC6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KD6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KE6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KF6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KG6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KH6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KI6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KJ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KK6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KL6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KM6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KN6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KO6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KP6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KT6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KU6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KV6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KW6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KX6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KY6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="KZ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LA6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LB6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LC6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LD6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LE6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LF6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LG6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LH6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LI6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LJ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LK6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LL6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LM6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LN6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LO6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LP6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LT6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LU6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LV6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LW6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LX6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LY6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="LZ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MA6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MB6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MC6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MD6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="ME6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MF6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MG6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MH6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MI6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MJ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MK6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="ML6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MM6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MN6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MO6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MP6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MT6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MU6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MV6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MW6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MX6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MY6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="MZ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NA6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NB6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NC6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="ND6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NE6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NF6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NG6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NH6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NI6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NJ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NK6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NL6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NM6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NN6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NO6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NP6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NT6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NU6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NV6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NW6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NX6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NY6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="NZ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OA6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OB6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OC6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OD6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OE6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OF6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OG6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OH6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OI6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OJ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OK6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OL6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OM6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="ON6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OO6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OP6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OT6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OU6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OV6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OW6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OX6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OY6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="OZ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PA6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PB6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PC6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PD6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PE6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PF6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PG6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PH6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PI6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PJ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PK6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PL6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PM6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PN6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PO6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PP6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PT6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PU6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PV6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PW6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PX6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PY6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="PZ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QA6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QB6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QC6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QD6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QE6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QF6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QG6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QH6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QI6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QJ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QK6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QL6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QM6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QN6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QO6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QP6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QT6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QU6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QV6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QW6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QX6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QY6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="QZ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RA6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RB6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RC6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RD6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RE6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RF6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RG6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RH6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RI6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RJ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RK6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RL6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RM6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RN6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RO6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RP6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RT6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RU6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RV6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RW6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RX6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RY6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="RZ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SA6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SB6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SC6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SD6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SE6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SF6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SG6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SH6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SI6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SJ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SK6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SL6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SM6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SN6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SO6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SP6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SQ6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SR6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="SS6" s="140" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:513">
       <c r="A9" s="155" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:513">
@@ -36241,10 +36240,10 @@
     </row>
     <row r="12" spans="1:513">
       <c r="A12" s="140" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B12" s="140" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C12" s="140">
         <f>C6/C5</f>
@@ -37241,10 +37240,10 @@
     </row>
     <row r="14" spans="1:513">
       <c r="A14" s="140" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B14" s="140" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C14" s="140">
         <f>AVERAGE(DZ12:IP12)</f>
@@ -37253,10 +37252,10 @@
     </row>
     <row r="16" spans="1:513">
       <c r="A16" s="140" t="s">
+        <v>245</v>
+      </c>
+      <c r="B16" s="148" t="s">
         <v>246</v>
-      </c>
-      <c r="B16" s="148" t="s">
-        <v>247</v>
       </c>
       <c r="C16" s="166">
         <f>C14*'[2]Field Crops'!R107</f>
@@ -37265,10 +37264,10 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="148" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B17" s="148" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C17" s="166">
         <f>C14*'[2]Field Crops'!R111</f>

</xml_diff>

<commit_message>
Working on Calculating Area of Land Required per head of Livestock
</commit_message>
<xml_diff>
--- a/LIVESTOCK-DATA-ORGANIZATION.xlsx
+++ b/LIVESTOCK-DATA-ORGANIZATION.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="260" yWindow="760" windowWidth="28740" windowHeight="17900" tabRatio="500" firstSheet="2" activeTab="8"/>
+    <workbookView xWindow="800" yWindow="40" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="2" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Feed Requ's Data" sheetId="4" r:id="rId1"/>
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="275">
   <si>
     <t>Tonnes/Head (Individual Livestock) Adjusted to Include Mill Screen Factor</t>
   </si>
@@ -974,12 +974,6 @@
     <t>Dry Peas - need to take av</t>
   </si>
   <si>
-    <t>Soybean Meal - soybeans?</t>
-  </si>
-  <si>
-    <t>result of previous….</t>
-  </si>
-  <si>
     <t>STATIC</t>
   </si>
   <si>
@@ -1002,6 +996,18 @@
   </si>
   <si>
     <t>turkey -  evicerated weight</t>
+  </si>
+  <si>
+    <t>RESULT</t>
+  </si>
+  <si>
+    <t>Pasture - 4 DM/hectare</t>
+  </si>
+  <si>
+    <t>Hay - 'tame hay'</t>
+  </si>
+  <si>
+    <t>Soybean Meal - (meal/seed crushed) ~ 0.775706681 incorrect currently getting .056</t>
   </si>
 </sst>
 </file>
@@ -1495,7 +1501,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="85">
+  <cellStyleXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1581,8 +1587,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="228">
+  <cellXfs count="226">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1847,14 +1861,22 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="17" fontId="11" fillId="6" borderId="0" xfId="38" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1863,15 +1885,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1906,9 +1919,8 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="11" fillId="6" borderId="0" xfId="38" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="85">
+  <cellStyles count="93">
     <cellStyle name="Comma 2" xfId="32"/>
     <cellStyle name="Comma 3" xfId="34"/>
     <cellStyle name="Comma 4" xfId="35"/>
@@ -1948,6 +1960,10 @@
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1980,6 +1996,10 @@
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="38"/>
     <cellStyle name="Normal 2" xfId="39"/>
@@ -5115,11 +5135,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2129015640"/>
-        <c:axId val="2129065784"/>
+        <c:axId val="2105394840"/>
+        <c:axId val="2105397816"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2129015640"/>
+        <c:axId val="2105394840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5129,14 +5149,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129065784"/>
+        <c:crossAx val="2105397816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2129065784"/>
+        <c:axId val="2105397816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5147,7 +5167,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2129015640"/>
+        <c:crossAx val="2105394840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7651,11 +7671,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2123895304"/>
-        <c:axId val="-2123892328"/>
+        <c:axId val="2103525352"/>
+        <c:axId val="2103522360"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2123895304"/>
+        <c:axId val="2103525352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7665,14 +7685,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123892328"/>
+        <c:crossAx val="2103522360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2123892328"/>
+        <c:axId val="2103522360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7683,7 +7703,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2123895304"/>
+        <c:crossAx val="2103525352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9239,11 +9259,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2124495464"/>
-        <c:axId val="-2105288536"/>
+        <c:axId val="2103502872"/>
+        <c:axId val="2103499880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="-2124495464"/>
+        <c:axId val="2103502872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9253,14 +9273,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2105288536"/>
+        <c:crossAx val="2103499880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="-2105288536"/>
+        <c:axId val="2103499880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9271,7 +9291,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124495464"/>
+        <c:crossAx val="2103502872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10311,7 +10331,7 @@
       <sheetName val="cansim-0010010-canola CND"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="107">
           <cell r="C107">
@@ -10332,17 +10352,17 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
       <sheetData sheetId="13">
         <row r="34">
           <cell r="D34">
@@ -10734,19 +10754,19 @@
       <c r="Z5" s="93"/>
     </row>
     <row r="6" spans="2:26" ht="14">
-      <c r="B6" s="210" t="s">
+      <c r="B6" s="212" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="211"/>
-      <c r="D6" s="211"/>
-      <c r="E6" s="211"/>
-      <c r="F6" s="211"/>
-      <c r="G6" s="211"/>
-      <c r="H6" s="211"/>
-      <c r="I6" s="211"/>
-      <c r="J6" s="211"/>
-      <c r="K6" s="211"/>
-      <c r="L6" s="212"/>
+      <c r="C6" s="213"/>
+      <c r="D6" s="213"/>
+      <c r="E6" s="213"/>
+      <c r="F6" s="213"/>
+      <c r="G6" s="213"/>
+      <c r="H6" s="213"/>
+      <c r="I6" s="213"/>
+      <c r="J6" s="213"/>
+      <c r="K6" s="213"/>
+      <c r="L6" s="214"/>
       <c r="M6" s="94"/>
       <c r="U6" s="93"/>
       <c r="V6" s="93"/>
@@ -10857,31 +10877,31 @@
     </row>
     <row r="10" spans="2:26" ht="13" thickBot="1"/>
     <row r="11" spans="2:26" ht="14">
-      <c r="B11" s="210" t="s">
+      <c r="B11" s="212" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="211"/>
-      <c r="D11" s="211"/>
-      <c r="E11" s="211"/>
-      <c r="F11" s="211"/>
-      <c r="G11" s="211"/>
-      <c r="H11" s="211"/>
-      <c r="I11" s="211"/>
-      <c r="J11" s="211"/>
-      <c r="K11" s="211"/>
-      <c r="L11" s="211"/>
-      <c r="M11" s="211"/>
-      <c r="N11" s="211"/>
-      <c r="O11" s="212"/>
-      <c r="P11" s="210" t="s">
+      <c r="C11" s="213"/>
+      <c r="D11" s="213"/>
+      <c r="E11" s="213"/>
+      <c r="F11" s="213"/>
+      <c r="G11" s="213"/>
+      <c r="H11" s="213"/>
+      <c r="I11" s="213"/>
+      <c r="J11" s="213"/>
+      <c r="K11" s="213"/>
+      <c r="L11" s="213"/>
+      <c r="M11" s="213"/>
+      <c r="N11" s="213"/>
+      <c r="O11" s="214"/>
+      <c r="P11" s="212" t="s">
         <v>84</v>
       </c>
-      <c r="Q11" s="211"/>
-      <c r="R11" s="211"/>
-      <c r="S11" s="211"/>
-      <c r="T11" s="211"/>
-      <c r="U11" s="211"/>
-      <c r="V11" s="212"/>
+      <c r="Q11" s="213"/>
+      <c r="R11" s="213"/>
+      <c r="S11" s="213"/>
+      <c r="T11" s="213"/>
+      <c r="U11" s="213"/>
+      <c r="V11" s="214"/>
     </row>
     <row r="12" spans="2:26" ht="14">
       <c r="B12" s="63" t="s">
@@ -12214,19 +12234,19 @@
       <c r="B30" s="31"/>
     </row>
     <row r="31" spans="2:24" s="80" customFormat="1" ht="14">
-      <c r="B31" s="210" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="211"/>
-      <c r="D31" s="211"/>
-      <c r="E31" s="211"/>
-      <c r="F31" s="211"/>
-      <c r="G31" s="211"/>
-      <c r="H31" s="211"/>
-      <c r="I31" s="211"/>
-      <c r="J31" s="211"/>
-      <c r="K31" s="211"/>
-      <c r="L31" s="212"/>
+      <c r="B31" s="212" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="213"/>
+      <c r="D31" s="213"/>
+      <c r="E31" s="213"/>
+      <c r="F31" s="213"/>
+      <c r="G31" s="213"/>
+      <c r="H31" s="213"/>
+      <c r="I31" s="213"/>
+      <c r="J31" s="213"/>
+      <c r="K31" s="213"/>
+      <c r="L31" s="214"/>
       <c r="M31" s="31"/>
       <c r="O31" s="31"/>
       <c r="P31" s="31"/>
@@ -13082,20 +13102,20 @@
       <c r="M50" s="83"/>
     </row>
     <row r="51" spans="2:20" s="80" customFormat="1" ht="14">
-      <c r="B51" s="210" t="s">
+      <c r="B51" s="212" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="211"/>
-      <c r="D51" s="211"/>
-      <c r="E51" s="211"/>
-      <c r="F51" s="211"/>
-      <c r="G51" s="211"/>
-      <c r="H51" s="211"/>
-      <c r="I51" s="211"/>
-      <c r="J51" s="211"/>
-      <c r="K51" s="211"/>
-      <c r="L51" s="211"/>
-      <c r="M51" s="212"/>
+      <c r="C51" s="213"/>
+      <c r="D51" s="213"/>
+      <c r="E51" s="213"/>
+      <c r="F51" s="213"/>
+      <c r="G51" s="213"/>
+      <c r="H51" s="213"/>
+      <c r="I51" s="213"/>
+      <c r="J51" s="213"/>
+      <c r="K51" s="213"/>
+      <c r="L51" s="213"/>
+      <c r="M51" s="214"/>
       <c r="O51" s="31"/>
     </row>
     <row r="52" spans="2:20" s="80" customFormat="1" ht="14">
@@ -14039,13 +14059,13 @@
       <c r="P71" s="34"/>
     </row>
     <row r="72" spans="2:25" ht="14">
-      <c r="B72" s="210" t="s">
+      <c r="B72" s="212" t="s">
         <v>80</v>
       </c>
-      <c r="C72" s="211"/>
-      <c r="D72" s="211"/>
-      <c r="E72" s="211"/>
-      <c r="F72" s="211"/>
+      <c r="C72" s="213"/>
+      <c r="D72" s="213"/>
+      <c r="E72" s="213"/>
+      <c r="F72" s="213"/>
       <c r="G72" s="64"/>
       <c r="K72" s="68"/>
     </row>
@@ -14366,13 +14386,13 @@
       <c r="K82" s="67"/>
     </row>
     <row r="83" spans="2:21" ht="14">
-      <c r="B83" s="210" t="s">
+      <c r="B83" s="212" t="s">
         <v>77</v>
       </c>
-      <c r="C83" s="211"/>
-      <c r="D83" s="211"/>
-      <c r="E83" s="211"/>
-      <c r="F83" s="211"/>
+      <c r="C83" s="213"/>
+      <c r="D83" s="213"/>
+      <c r="E83" s="213"/>
+      <c r="F83" s="213"/>
       <c r="G83" s="66"/>
       <c r="H83" s="66"/>
       <c r="I83" s="65" t="s">
@@ -14679,11 +14699,11 @@
       <c r="P93" s="34"/>
     </row>
     <row r="94" spans="2:21" ht="14">
-      <c r="B94" s="213" t="s">
+      <c r="B94" s="209" t="s">
         <v>69</v>
       </c>
-      <c r="C94" s="214"/>
-      <c r="D94" s="215"/>
+      <c r="C94" s="210"/>
+      <c r="D94" s="211"/>
       <c r="E94" s="42"/>
       <c r="F94" s="34"/>
       <c r="G94" s="41"/>
@@ -14912,14 +14932,14 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
-    <mergeCell ref="P11:V11"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B83:F83"/>
     <mergeCell ref="B6:L6"/>
     <mergeCell ref="B51:M51"/>
     <mergeCell ref="B31:L31"/>
     <mergeCell ref="B94:D94"/>
     <mergeCell ref="B11:O11"/>
+    <mergeCell ref="P11:V11"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B83:F83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -15850,19 +15870,19 @@
     </row>
     <row r="20" spans="1:14" ht="16" thickBot="1"/>
     <row r="21" spans="1:14">
-      <c r="A21" s="216" t="s">
+      <c r="A21" s="215" t="s">
         <v>57</v>
       </c>
-      <c r="B21" s="217"/>
-      <c r="C21" s="217"/>
-      <c r="D21" s="217"/>
-      <c r="E21" s="217"/>
-      <c r="F21" s="217"/>
-      <c r="G21" s="217"/>
-      <c r="H21" s="217"/>
-      <c r="I21" s="217"/>
-      <c r="J21" s="217"/>
-      <c r="K21" s="218"/>
+      <c r="B21" s="216"/>
+      <c r="C21" s="216"/>
+      <c r="D21" s="216"/>
+      <c r="E21" s="216"/>
+      <c r="F21" s="216"/>
+      <c r="G21" s="216"/>
+      <c r="H21" s="216"/>
+      <c r="I21" s="216"/>
+      <c r="J21" s="216"/>
+      <c r="K21" s="217"/>
     </row>
     <row r="22" spans="1:14">
       <c r="A22" s="20" t="s">
@@ -17384,8 +17404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA55"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="N34" sqref="N34"/>
+    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17726,22 +17746,24 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
       <c r="H25" s="198" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="I25" s="15"/>
       <c r="J25" s="181" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="K25" s="15"/>
       <c r="L25" s="181" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="M25" s="15"/>
       <c r="N25" s="182" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="O25" s="15"/>
-      <c r="P25" s="197"/>
+      <c r="P25" s="181" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="26" spans="1:27">
       <c r="H26" s="196"/>
@@ -17801,13 +17823,17 @@
         <v>2</v>
       </c>
       <c r="K28" s="15"/>
-      <c r="L28" s="185"/>
+      <c r="L28" s="201" t="s">
+        <v>38</v>
+      </c>
       <c r="M28" s="15"/>
       <c r="N28" s="185" t="s">
         <v>133</v>
       </c>
       <c r="O28" s="15"/>
-      <c r="P28" s="202"/>
+      <c r="P28" s="201" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="29" spans="1:27">
       <c r="A29" s="8"/>
@@ -17834,8 +17860,8 @@
       <c r="K29" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="L29" s="185" t="s">
-        <v>264</v>
+      <c r="L29" s="201" t="s">
+        <v>271</v>
       </c>
       <c r="M29" s="15" t="s">
         <v>128</v>
@@ -17846,7 +17872,9 @@
       <c r="O29" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="P29" s="202"/>
+      <c r="P29" s="201" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="30" spans="1:27">
       <c r="A30" s="8"/>
@@ -17869,13 +17897,17 @@
         <v>4</v>
       </c>
       <c r="K30" s="15"/>
-      <c r="L30" s="185"/>
+      <c r="L30" s="201" t="s">
+        <v>38</v>
+      </c>
       <c r="M30" s="15"/>
       <c r="N30" s="185" t="s">
         <v>135</v>
       </c>
       <c r="O30" s="15"/>
-      <c r="P30" s="202"/>
+      <c r="P30" s="201" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="31" spans="1:27">
       <c r="A31" s="8"/>
@@ -17898,13 +17930,17 @@
         <v>5</v>
       </c>
       <c r="K31" s="15"/>
-      <c r="L31" s="185"/>
+      <c r="L31" s="201" t="s">
+        <v>38</v>
+      </c>
       <c r="M31" s="15"/>
       <c r="N31" s="186" t="s">
         <v>136</v>
       </c>
       <c r="O31" s="15"/>
-      <c r="P31" s="202"/>
+      <c r="P31" s="201" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="32" spans="1:27">
       <c r="C32" s="10"/>
@@ -17917,8 +17953,8 @@
       <c r="K32" s="15"/>
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
-      <c r="N32" s="209" t="s">
-        <v>271</v>
+      <c r="N32" s="183" t="s">
+        <v>269</v>
       </c>
       <c r="O32" s="15"/>
       <c r="P32" s="197"/>
@@ -17927,13 +17963,13 @@
       <c r="H33" s="196"/>
       <c r="I33" s="15"/>
       <c r="J33" s="186" t="s">
-        <v>263</v>
+        <v>274</v>
       </c>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
-      <c r="N33" s="209" t="s">
-        <v>272</v>
+      <c r="N33" s="183" t="s">
+        <v>270</v>
       </c>
       <c r="O33" s="15"/>
       <c r="P33" s="197"/>
@@ -17941,7 +17977,7 @@
     <row r="34" spans="2:16">
       <c r="H34" s="196"/>
       <c r="I34" s="15"/>
-      <c r="J34" s="186" t="s">
+      <c r="J34" s="184" t="s">
         <v>8</v>
       </c>
       <c r="K34" s="15"/>
@@ -17957,7 +17993,7 @@
       <c r="H35" s="196"/>
       <c r="I35" s="15"/>
       <c r="J35" s="184" t="s">
-        <v>9</v>
+        <v>272</v>
       </c>
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
@@ -17973,17 +18009,17 @@
       <c r="E36" s="8"/>
       <c r="F36" s="8"/>
       <c r="G36" s="8"/>
-      <c r="H36" s="203"/>
+      <c r="H36" s="202"/>
       <c r="I36" s="187"/>
-      <c r="J36" s="186" t="s">
-        <v>10</v>
+      <c r="J36" s="184" t="s">
+        <v>273</v>
       </c>
       <c r="K36" s="187"/>
       <c r="L36" s="187"/>
       <c r="M36" s="187"/>
       <c r="N36" s="187"/>
       <c r="O36" s="187"/>
-      <c r="P36" s="204"/>
+      <c r="P36" s="203"/>
     </row>
     <row r="37" spans="2:16">
       <c r="B37" s="9"/>
@@ -17992,7 +18028,7 @@
       <c r="E37" s="9"/>
       <c r="F37" s="9"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="205"/>
+      <c r="H37" s="204"/>
       <c r="I37" s="188"/>
       <c r="J37" s="186" t="s">
         <v>11</v>
@@ -18002,7 +18038,7 @@
       <c r="M37" s="188"/>
       <c r="N37" s="188"/>
       <c r="O37" s="188"/>
-      <c r="P37" s="204"/>
+      <c r="P37" s="203"/>
     </row>
     <row r="38" spans="2:16">
       <c r="B38" s="9"/>
@@ -18019,7 +18055,7 @@
       <c r="M38" s="187"/>
       <c r="N38" s="187"/>
       <c r="O38" s="187"/>
-      <c r="P38" s="204"/>
+      <c r="P38" s="203"/>
     </row>
     <row r="39" spans="2:16">
       <c r="B39" s="9"/>
@@ -18028,19 +18064,19 @@
       <c r="E39" s="8"/>
       <c r="F39" s="8"/>
       <c r="G39" s="8"/>
-      <c r="H39" s="203"/>
+      <c r="H39" s="202"/>
       <c r="I39" s="187"/>
       <c r="J39" s="190" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="K39" s="187"/>
       <c r="L39" s="187"/>
       <c r="M39" s="187"/>
       <c r="N39" s="191" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="O39" s="187"/>
-      <c r="P39" s="204"/>
+      <c r="P39" s="203"/>
     </row>
     <row r="40" spans="2:16">
       <c r="B40" s="9"/>
@@ -18049,17 +18085,17 @@
       <c r="E40" s="8"/>
       <c r="F40" s="8"/>
       <c r="G40" s="8"/>
-      <c r="H40" s="203"/>
+      <c r="H40" s="202"/>
       <c r="I40" s="187"/>
       <c r="J40" s="192" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="K40" s="187"/>
       <c r="L40" s="187"/>
       <c r="M40" s="187"/>
       <c r="N40" s="192"/>
       <c r="O40" s="187"/>
-      <c r="P40" s="204"/>
+      <c r="P40" s="203"/>
     </row>
     <row r="41" spans="2:16">
       <c r="B41" s="9"/>
@@ -18068,7 +18104,7 @@
       <c r="E41" s="8"/>
       <c r="F41" s="8"/>
       <c r="G41" s="8"/>
-      <c r="H41" s="203"/>
+      <c r="H41" s="202"/>
       <c r="I41" s="187"/>
       <c r="J41" s="15"/>
       <c r="K41" s="187"/>
@@ -18076,7 +18112,7 @@
       <c r="M41" s="187"/>
       <c r="N41" s="187"/>
       <c r="O41" s="187"/>
-      <c r="P41" s="204"/>
+      <c r="P41" s="203"/>
     </row>
     <row r="42" spans="2:16">
       <c r="B42" s="9"/>
@@ -18085,17 +18121,17 @@
       <c r="E42" s="8"/>
       <c r="F42" s="8"/>
       <c r="G42" s="8"/>
-      <c r="H42" s="203"/>
+      <c r="H42" s="202"/>
       <c r="I42" s="187"/>
       <c r="J42" s="191" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="K42" s="187"/>
       <c r="L42" s="187"/>
       <c r="M42" s="187"/>
       <c r="N42" s="187"/>
       <c r="O42" s="187"/>
-      <c r="P42" s="204"/>
+      <c r="P42" s="203"/>
     </row>
     <row r="43" spans="2:16">
       <c r="B43" s="9"/>
@@ -18104,7 +18140,7 @@
       <c r="E43" s="8"/>
       <c r="F43" s="8"/>
       <c r="G43" s="8"/>
-      <c r="H43" s="203"/>
+      <c r="H43" s="202"/>
       <c r="I43" s="187"/>
       <c r="J43" s="192"/>
       <c r="K43" s="187"/>
@@ -18112,7 +18148,7 @@
       <c r="M43" s="187"/>
       <c r="N43" s="187"/>
       <c r="O43" s="187"/>
-      <c r="P43" s="204"/>
+      <c r="P43" s="203"/>
     </row>
     <row r="44" spans="2:16">
       <c r="B44" s="9"/>
@@ -18121,7 +18157,7 @@
       <c r="E44" s="8"/>
       <c r="F44" s="8"/>
       <c r="G44" s="8"/>
-      <c r="H44" s="203"/>
+      <c r="H44" s="202"/>
       <c r="I44" s="187"/>
       <c r="J44" s="187"/>
       <c r="K44" s="187"/>
@@ -18129,7 +18165,7 @@
       <c r="M44" s="187"/>
       <c r="N44" s="187"/>
       <c r="O44" s="187"/>
-      <c r="P44" s="204"/>
+      <c r="P44" s="203"/>
     </row>
     <row r="45" spans="2:16" ht="16" thickBot="1">
       <c r="B45" s="9"/>
@@ -18138,15 +18174,15 @@
       <c r="E45" s="8"/>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
-      <c r="H45" s="206"/>
-      <c r="I45" s="207"/>
-      <c r="J45" s="207"/>
-      <c r="K45" s="207"/>
-      <c r="L45" s="207"/>
-      <c r="M45" s="207"/>
-      <c r="N45" s="207"/>
-      <c r="O45" s="207"/>
-      <c r="P45" s="208"/>
+      <c r="H45" s="205"/>
+      <c r="I45" s="206"/>
+      <c r="J45" s="206"/>
+      <c r="K45" s="206"/>
+      <c r="L45" s="206"/>
+      <c r="M45" s="206"/>
+      <c r="N45" s="206"/>
+      <c r="O45" s="206"/>
+      <c r="P45" s="207"/>
     </row>
     <row r="46" spans="2:16">
       <c r="B46" s="9"/>
@@ -18985,7 +19021,7 @@
   <dimension ref="A1:S112"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B97" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="B82" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
       <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
@@ -19037,28 +19073,28 @@
       <c r="D3" s="155"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="B4" s="219" t="s">
+      <c r="B4" s="218" t="s">
         <v>198</v>
       </c>
-      <c r="C4" s="219"/>
-      <c r="D4" s="219"/>
-      <c r="E4" s="219"/>
-      <c r="F4" s="219"/>
-      <c r="G4" s="219"/>
-      <c r="H4" s="219"/>
-      <c r="I4" s="219"/>
-      <c r="J4" s="219"/>
-      <c r="K4" s="219"/>
-      <c r="L4" s="219"/>
-      <c r="M4" s="219"/>
-      <c r="N4" s="219"/>
-      <c r="O4" s="219"/>
-      <c r="P4" s="220"/>
-      <c r="Q4" s="221" t="s">
+      <c r="C4" s="218"/>
+      <c r="D4" s="218"/>
+      <c r="E4" s="218"/>
+      <c r="F4" s="218"/>
+      <c r="G4" s="218"/>
+      <c r="H4" s="218"/>
+      <c r="I4" s="218"/>
+      <c r="J4" s="218"/>
+      <c r="K4" s="218"/>
+      <c r="L4" s="218"/>
+      <c r="M4" s="218"/>
+      <c r="N4" s="218"/>
+      <c r="O4" s="218"/>
+      <c r="P4" s="219"/>
+      <c r="Q4" s="220" t="s">
         <v>199</v>
       </c>
-      <c r="R4" s="222"/>
-      <c r="S4" s="222"/>
+      <c r="R4" s="221"/>
+      <c r="S4" s="221"/>
     </row>
     <row r="5" spans="1:19" s="156" customFormat="1" ht="46.5" customHeight="1">
       <c r="B5" s="156" t="s">
@@ -24580,16 +24616,16 @@
         <v>9.3715821862348196</v>
       </c>
       <c r="C22" s="115"/>
-      <c r="D22" s="223" t="s">
+      <c r="D22" s="222" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="224"/>
-      <c r="F22" s="224"/>
-      <c r="G22" s="224"/>
-      <c r="H22" s="224"/>
-      <c r="I22" s="224"/>
-      <c r="J22" s="224"/>
-      <c r="K22" s="224"/>
+      <c r="E22" s="223"/>
+      <c r="F22" s="223"/>
+      <c r="G22" s="223"/>
+      <c r="H22" s="223"/>
+      <c r="I22" s="223"/>
+      <c r="J22" s="223"/>
+      <c r="K22" s="223"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="125" t="s">
@@ -24600,14 +24636,14 @@
         <v>2.916666666666667</v>
       </c>
       <c r="C23" s="119"/>
-      <c r="D23" s="223"/>
-      <c r="E23" s="224"/>
-      <c r="F23" s="224"/>
-      <c r="G23" s="224"/>
-      <c r="H23" s="224"/>
-      <c r="I23" s="224"/>
-      <c r="J23" s="224"/>
-      <c r="K23" s="224"/>
+      <c r="D23" s="222"/>
+      <c r="E23" s="223"/>
+      <c r="F23" s="223"/>
+      <c r="G23" s="223"/>
+      <c r="H23" s="223"/>
+      <c r="I23" s="223"/>
+      <c r="J23" s="223"/>
+      <c r="K23" s="223"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="101" t="s">
@@ -24705,16 +24741,16 @@
         <v>57.243045490211102</v>
       </c>
       <c r="C30" s="119"/>
-      <c r="D30" s="223" t="s">
+      <c r="D30" s="222" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="224"/>
-      <c r="F30" s="224"/>
-      <c r="G30" s="224"/>
-      <c r="H30" s="224"/>
-      <c r="I30" s="224"/>
-      <c r="J30" s="224"/>
-      <c r="K30" s="224"/>
+      <c r="E30" s="223"/>
+      <c r="F30" s="223"/>
+      <c r="G30" s="223"/>
+      <c r="H30" s="223"/>
+      <c r="I30" s="223"/>
+      <c r="J30" s="223"/>
+      <c r="K30" s="223"/>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="116" t="s">
@@ -24725,14 +24761,14 @@
         <v>0.16371564625850341</v>
       </c>
       <c r="C31" s="119"/>
-      <c r="D31" s="223"/>
-      <c r="E31" s="224"/>
-      <c r="F31" s="224"/>
-      <c r="G31" s="224"/>
-      <c r="H31" s="224"/>
-      <c r="I31" s="224"/>
-      <c r="J31" s="224"/>
-      <c r="K31" s="224"/>
+      <c r="D31" s="222"/>
+      <c r="E31" s="223"/>
+      <c r="F31" s="223"/>
+      <c r="G31" s="223"/>
+      <c r="H31" s="223"/>
+      <c r="I31" s="223"/>
+      <c r="J31" s="223"/>
+      <c r="K31" s="223"/>
     </row>
     <row r="32" spans="1:11">
       <c r="F32">
@@ -24801,7 +24837,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView topLeftCell="A38" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -24829,11 +24865,11 @@
       <c r="A3" s="152" t="s">
         <v>192</v>
       </c>
-      <c r="B3" s="225" t="s">
+      <c r="B3" s="224" t="s">
         <v>191</v>
       </c>
-      <c r="C3" s="225"/>
-      <c r="D3" s="225"/>
+      <c r="C3" s="224"/>
+      <c r="D3" s="224"/>
       <c r="E3" s="152" t="s">
         <v>190</v>
       </c>
@@ -25024,17 +25060,17 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="226" t="s">
+      <c r="A27" s="225" t="s">
         <v>165</v>
       </c>
-      <c r="B27" s="226"/>
-      <c r="C27" s="226"/>
-      <c r="D27" s="226"/>
-      <c r="E27" s="226"/>
-      <c r="F27" s="226"/>
-      <c r="G27" s="226"/>
-      <c r="H27" s="226"/>
-      <c r="I27" s="226"/>
+      <c r="B27" s="225"/>
+      <c r="C27" s="225"/>
+      <c r="D27" s="225"/>
+      <c r="E27" s="225"/>
+      <c r="F27" s="225"/>
+      <c r="G27" s="225"/>
+      <c r="H27" s="225"/>
+      <c r="I27" s="225"/>
     </row>
     <row r="28" spans="1:9" s="148" customFormat="1">
       <c r="A28" s="147"/>
@@ -38176,8 +38212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:SS17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="HQ3" workbookViewId="0">
-      <selection activeCell="DZ4" sqref="DZ4:IP6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -38590,7 +38626,7 @@
       <c r="DY4" s="165">
         <v>29983</v>
       </c>
-      <c r="DZ4" s="227">
+      <c r="DZ4" s="208">
         <v>30011</v>
       </c>
       <c r="EA4" s="165">
@@ -38950,7 +38986,7 @@
       <c r="IO4" s="165">
         <v>33635</v>
       </c>
-      <c r="IP4" s="227">
+      <c r="IP4" s="208">
         <v>33664</v>
       </c>
       <c r="IQ4" s="165">
@@ -43233,7 +43269,7 @@
       <c r="DY11" s="165">
         <v>29983</v>
       </c>
-      <c r="DZ11" s="227">
+      <c r="DZ11" s="208">
         <v>30011</v>
       </c>
       <c r="EA11" s="165">
@@ -43593,7 +43629,7 @@
       <c r="IO11" s="165">
         <v>33635</v>
       </c>
-      <c r="IP11" s="227">
+      <c r="IP11" s="208">
         <v>33664</v>
       </c>
     </row>
@@ -44635,6 +44671,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
calculating land area for livestock
</commit_message>
<xml_diff>
--- a/LIVESTOCK-DATA-ORGANIZATION.xlsx
+++ b/LIVESTOCK-DATA-ORGANIZATION.xlsx
@@ -170,7 +170,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="274">
   <si>
     <t>Tonnes/Head (Individual Livestock) Adjusted to Include Mill Screen Factor</t>
   </si>
@@ -986,9 +986,6 @@
     <t>if no BC use Canada data</t>
   </si>
   <si>
-    <t>canola and soy meal yield</t>
-  </si>
-  <si>
     <t>chicken/turkey calc?</t>
   </si>
   <si>
@@ -1007,7 +1004,7 @@
     <t>Hay - 'tame hay'</t>
   </si>
   <si>
-    <t>Soybean Meal - (meal/seed crushed) ~ 0.775706681 incorrect currently getting .056</t>
+    <t>Soybean Meal - static value</t>
   </si>
 </sst>
 </file>
@@ -1501,7 +1498,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1595,8 +1592,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="226">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1869,6 +1872,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="11" fillId="6" borderId="0" xfId="38" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1876,15 +1888,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1919,8 +1922,9 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="7" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="99">
     <cellStyle name="Comma 2" xfId="32"/>
     <cellStyle name="Comma 3" xfId="34"/>
     <cellStyle name="Comma 4" xfId="35"/>
@@ -1964,6 +1968,9 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2000,6 +2007,9 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="38"/>
     <cellStyle name="Normal 2" xfId="39"/>
@@ -5135,11 +5145,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2105394840"/>
-        <c:axId val="2105397816"/>
+        <c:axId val="2129117608"/>
+        <c:axId val="2129117960"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2105394840"/>
+        <c:axId val="2129117608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5149,14 +5159,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105397816"/>
+        <c:crossAx val="2129117960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2105397816"/>
+        <c:axId val="2129117960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5167,7 +5177,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2105394840"/>
+        <c:crossAx val="2129117608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7671,11 +7681,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2103525352"/>
-        <c:axId val="2103522360"/>
+        <c:axId val="2129220520"/>
+        <c:axId val="2129223496"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2103525352"/>
+        <c:axId val="2129220520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7685,14 +7695,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103522360"/>
+        <c:crossAx val="2129223496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2103522360"/>
+        <c:axId val="2129223496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7703,7 +7713,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103525352"/>
+        <c:crossAx val="2129220520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9259,11 +9269,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2103502872"/>
-        <c:axId val="2103499880"/>
+        <c:axId val="2081048328"/>
+        <c:axId val="2081051304"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2103502872"/>
+        <c:axId val="2081048328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9273,14 +9283,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103499880"/>
+        <c:crossAx val="2081051304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2103499880"/>
+        <c:axId val="2081051304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9291,7 +9301,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2103502872"/>
+        <c:crossAx val="2081048328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10754,19 +10764,19 @@
       <c r="Z5" s="93"/>
     </row>
     <row r="6" spans="2:26" ht="14">
-      <c r="B6" s="212" t="s">
+      <c r="B6" s="209" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="213"/>
-      <c r="D6" s="213"/>
-      <c r="E6" s="213"/>
-      <c r="F6" s="213"/>
-      <c r="G6" s="213"/>
-      <c r="H6" s="213"/>
-      <c r="I6" s="213"/>
-      <c r="J6" s="213"/>
-      <c r="K6" s="213"/>
-      <c r="L6" s="214"/>
+      <c r="C6" s="210"/>
+      <c r="D6" s="210"/>
+      <c r="E6" s="210"/>
+      <c r="F6" s="210"/>
+      <c r="G6" s="210"/>
+      <c r="H6" s="210"/>
+      <c r="I6" s="210"/>
+      <c r="J6" s="210"/>
+      <c r="K6" s="210"/>
+      <c r="L6" s="211"/>
       <c r="M6" s="94"/>
       <c r="U6" s="93"/>
       <c r="V6" s="93"/>
@@ -10877,31 +10887,31 @@
     </row>
     <row r="10" spans="2:26" ht="13" thickBot="1"/>
     <row r="11" spans="2:26" ht="14">
-      <c r="B11" s="212" t="s">
+      <c r="B11" s="209" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="213"/>
-      <c r="D11" s="213"/>
-      <c r="E11" s="213"/>
-      <c r="F11" s="213"/>
-      <c r="G11" s="213"/>
-      <c r="H11" s="213"/>
-      <c r="I11" s="213"/>
-      <c r="J11" s="213"/>
-      <c r="K11" s="213"/>
-      <c r="L11" s="213"/>
-      <c r="M11" s="213"/>
-      <c r="N11" s="213"/>
-      <c r="O11" s="214"/>
-      <c r="P11" s="212" t="s">
+      <c r="C11" s="210"/>
+      <c r="D11" s="210"/>
+      <c r="E11" s="210"/>
+      <c r="F11" s="210"/>
+      <c r="G11" s="210"/>
+      <c r="H11" s="210"/>
+      <c r="I11" s="210"/>
+      <c r="J11" s="210"/>
+      <c r="K11" s="210"/>
+      <c r="L11" s="210"/>
+      <c r="M11" s="210"/>
+      <c r="N11" s="210"/>
+      <c r="O11" s="211"/>
+      <c r="P11" s="209" t="s">
         <v>84</v>
       </c>
-      <c r="Q11" s="213"/>
-      <c r="R11" s="213"/>
-      <c r="S11" s="213"/>
-      <c r="T11" s="213"/>
-      <c r="U11" s="213"/>
-      <c r="V11" s="214"/>
+      <c r="Q11" s="210"/>
+      <c r="R11" s="210"/>
+      <c r="S11" s="210"/>
+      <c r="T11" s="210"/>
+      <c r="U11" s="210"/>
+      <c r="V11" s="211"/>
     </row>
     <row r="12" spans="2:26" ht="14">
       <c r="B12" s="63" t="s">
@@ -12234,19 +12244,19 @@
       <c r="B30" s="31"/>
     </row>
     <row r="31" spans="2:24" s="80" customFormat="1" ht="14">
-      <c r="B31" s="212" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="213"/>
-      <c r="D31" s="213"/>
-      <c r="E31" s="213"/>
-      <c r="F31" s="213"/>
-      <c r="G31" s="213"/>
-      <c r="H31" s="213"/>
-      <c r="I31" s="213"/>
-      <c r="J31" s="213"/>
-      <c r="K31" s="213"/>
-      <c r="L31" s="214"/>
+      <c r="B31" s="209" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="210"/>
+      <c r="D31" s="210"/>
+      <c r="E31" s="210"/>
+      <c r="F31" s="210"/>
+      <c r="G31" s="210"/>
+      <c r="H31" s="210"/>
+      <c r="I31" s="210"/>
+      <c r="J31" s="210"/>
+      <c r="K31" s="210"/>
+      <c r="L31" s="211"/>
       <c r="M31" s="31"/>
       <c r="O31" s="31"/>
       <c r="P31" s="31"/>
@@ -13102,20 +13112,20 @@
       <c r="M50" s="83"/>
     </row>
     <row r="51" spans="2:20" s="80" customFormat="1" ht="14">
-      <c r="B51" s="212" t="s">
+      <c r="B51" s="209" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="213"/>
-      <c r="D51" s="213"/>
-      <c r="E51" s="213"/>
-      <c r="F51" s="213"/>
-      <c r="G51" s="213"/>
-      <c r="H51" s="213"/>
-      <c r="I51" s="213"/>
-      <c r="J51" s="213"/>
-      <c r="K51" s="213"/>
-      <c r="L51" s="213"/>
-      <c r="M51" s="214"/>
+      <c r="C51" s="210"/>
+      <c r="D51" s="210"/>
+      <c r="E51" s="210"/>
+      <c r="F51" s="210"/>
+      <c r="G51" s="210"/>
+      <c r="H51" s="210"/>
+      <c r="I51" s="210"/>
+      <c r="J51" s="210"/>
+      <c r="K51" s="210"/>
+      <c r="L51" s="210"/>
+      <c r="M51" s="211"/>
       <c r="O51" s="31"/>
     </row>
     <row r="52" spans="2:20" s="80" customFormat="1" ht="14">
@@ -14059,13 +14069,13 @@
       <c r="P71" s="34"/>
     </row>
     <row r="72" spans="2:25" ht="14">
-      <c r="B72" s="212" t="s">
+      <c r="B72" s="209" t="s">
         <v>80</v>
       </c>
-      <c r="C72" s="213"/>
-      <c r="D72" s="213"/>
-      <c r="E72" s="213"/>
-      <c r="F72" s="213"/>
+      <c r="C72" s="210"/>
+      <c r="D72" s="210"/>
+      <c r="E72" s="210"/>
+      <c r="F72" s="210"/>
       <c r="G72" s="64"/>
       <c r="K72" s="68"/>
     </row>
@@ -14386,13 +14396,13 @@
       <c r="K82" s="67"/>
     </row>
     <row r="83" spans="2:21" ht="14">
-      <c r="B83" s="212" t="s">
+      <c r="B83" s="209" t="s">
         <v>77</v>
       </c>
-      <c r="C83" s="213"/>
-      <c r="D83" s="213"/>
-      <c r="E83" s="213"/>
-      <c r="F83" s="213"/>
+      <c r="C83" s="210"/>
+      <c r="D83" s="210"/>
+      <c r="E83" s="210"/>
+      <c r="F83" s="210"/>
       <c r="G83" s="66"/>
       <c r="H83" s="66"/>
       <c r="I83" s="65" t="s">
@@ -14699,11 +14709,11 @@
       <c r="P93" s="34"/>
     </row>
     <row r="94" spans="2:21" ht="14">
-      <c r="B94" s="209" t="s">
+      <c r="B94" s="212" t="s">
         <v>69</v>
       </c>
-      <c r="C94" s="210"/>
-      <c r="D94" s="211"/>
+      <c r="C94" s="213"/>
+      <c r="D94" s="214"/>
       <c r="E94" s="42"/>
       <c r="F94" s="34"/>
       <c r="G94" s="41"/>
@@ -14932,14 +14942,14 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="8">
+    <mergeCell ref="P11:V11"/>
+    <mergeCell ref="B72:F72"/>
+    <mergeCell ref="B83:F83"/>
     <mergeCell ref="B6:L6"/>
     <mergeCell ref="B51:M51"/>
     <mergeCell ref="B31:L31"/>
     <mergeCell ref="B94:D94"/>
     <mergeCell ref="B11:O11"/>
-    <mergeCell ref="P11:V11"/>
-    <mergeCell ref="B72:F72"/>
-    <mergeCell ref="B83:F83"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -17404,8 +17414,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AA55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E16" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" topLeftCell="F15" workbookViewId="0">
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17861,7 +17871,7 @@
         <v>129</v>
       </c>
       <c r="L29" s="201" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M29" s="15" t="s">
         <v>128</v>
@@ -17873,7 +17883,7 @@
         <v>129</v>
       </c>
       <c r="P29" s="201" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:27">
@@ -17954,7 +17964,7 @@
       <c r="L32" s="15"/>
       <c r="M32" s="15"/>
       <c r="N32" s="183" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O32" s="15"/>
       <c r="P32" s="197"/>
@@ -17962,14 +17972,14 @@
     <row r="33" spans="2:16">
       <c r="H33" s="196"/>
       <c r="I33" s="15"/>
-      <c r="J33" s="186" t="s">
-        <v>274</v>
+      <c r="J33" s="184" t="s">
+        <v>273</v>
       </c>
       <c r="K33" s="15"/>
       <c r="L33" s="15"/>
       <c r="M33" s="15"/>
       <c r="N33" s="183" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O33" s="15"/>
       <c r="P33" s="197"/>
@@ -17993,7 +18003,7 @@
       <c r="H35" s="196"/>
       <c r="I35" s="15"/>
       <c r="J35" s="184" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
@@ -18012,7 +18022,7 @@
       <c r="H36" s="202"/>
       <c r="I36" s="187"/>
       <c r="J36" s="184" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="K36" s="187"/>
       <c r="L36" s="187"/>
@@ -18073,7 +18083,7 @@
       <c r="L39" s="187"/>
       <c r="M39" s="187"/>
       <c r="N39" s="191" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="O39" s="187"/>
       <c r="P39" s="203"/>
@@ -18123,9 +18133,7 @@
       <c r="G42" s="8"/>
       <c r="H42" s="202"/>
       <c r="I42" s="187"/>
-      <c r="J42" s="191" t="s">
-        <v>267</v>
-      </c>
+      <c r="J42" s="226"/>
       <c r="K42" s="187"/>
       <c r="L42" s="187"/>
       <c r="M42" s="187"/>
@@ -18142,7 +18150,7 @@
       <c r="G43" s="8"/>
       <c r="H43" s="202"/>
       <c r="I43" s="187"/>
-      <c r="J43" s="192"/>
+      <c r="J43" s="187"/>
       <c r="K43" s="187"/>
       <c r="L43" s="187"/>
       <c r="M43" s="187"/>
@@ -24329,7 +24337,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="D22" sqref="D22:K35"/>
     </sheetView>
   </sheetViews>
@@ -24837,8 +24845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -38213,7 +38221,7 @@
   <dimension ref="A1:SS17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:C14"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
done done done for nowww
</commit_message>
<xml_diff>
--- a/LIVESTOCK-DATA-ORGANIZATION.xlsx
+++ b/LIVESTOCK-DATA-ORGANIZATION.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="0" windowWidth="24840" windowHeight="17660" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2380" yWindow="0" windowWidth="28540" windowHeight="17660" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Feed Requ's Data" sheetId="4" r:id="rId1"/>
@@ -247,7 +247,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1504" uniqueCount="317">
   <si>
     <t>Tonnes/Head (Individual Livestock) Adjusted to Include Mill Screen Factor</t>
   </si>
@@ -1190,6 +1190,27 @@
   <si>
     <t>GSM</t>
   </si>
+  <si>
+    <t>Lifespan of animal</t>
+  </si>
+  <si>
+    <t>Lifespan of breeder</t>
+  </si>
+  <si>
+    <t>Wo</t>
+  </si>
+  <si>
+    <t>Wb</t>
+  </si>
+  <si>
+    <t>Lb</t>
+  </si>
+  <si>
+    <t>noffspring</t>
+  </si>
+  <si>
+    <t>Fr</t>
+  </si>
 </sst>
 </file>
 
@@ -1349,7 +1370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1461,6 +1482,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1780,7 +1813,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="225">
+  <cellStyleXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2006,8 +2039,46 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="311">
+  <cellXfs count="325">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -2351,7 +2422,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="24" xfId="29" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="24" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="24" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="29" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="29" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="29" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2419,12 +2489,27 @@
     <xf numFmtId="0" fontId="14" fillId="17" borderId="27" xfId="29" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="27" xfId="29" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="29" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="29" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="29" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="225">
+  <cellStyles count="263">
     <cellStyle name="Comma 2" xfId="32"/>
     <cellStyle name="Comma 3" xfId="34"/>
     <cellStyle name="Comma 4" xfId="35"/>
@@ -2534,6 +2619,25 @@
     <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2636,6 +2740,25 @@
     <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 10" xfId="38"/>
     <cellStyle name="Normal 2" xfId="39"/>
@@ -11842,19 +11965,19 @@
       <c r="Z5" s="74"/>
     </row>
     <row r="6" spans="2:26" ht="14">
-      <c r="B6" s="279" t="s">
+      <c r="B6" s="278" t="s">
         <v>65</v>
       </c>
-      <c r="C6" s="280"/>
-      <c r="D6" s="280"/>
-      <c r="E6" s="280"/>
-      <c r="F6" s="280"/>
-      <c r="G6" s="280"/>
-      <c r="H6" s="280"/>
-      <c r="I6" s="280"/>
-      <c r="J6" s="280"/>
-      <c r="K6" s="280"/>
-      <c r="L6" s="281"/>
+      <c r="C6" s="279"/>
+      <c r="D6" s="279"/>
+      <c r="E6" s="279"/>
+      <c r="F6" s="279"/>
+      <c r="G6" s="279"/>
+      <c r="H6" s="279"/>
+      <c r="I6" s="279"/>
+      <c r="J6" s="279"/>
+      <c r="K6" s="279"/>
+      <c r="L6" s="280"/>
       <c r="M6" s="75"/>
       <c r="U6" s="74"/>
       <c r="V6" s="74"/>
@@ -11965,31 +12088,31 @@
     </row>
     <row r="10" spans="2:26" ht="13" thickBot="1"/>
     <row r="11" spans="2:26" ht="14">
-      <c r="B11" s="279" t="s">
+      <c r="B11" s="278" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="280"/>
-      <c r="D11" s="280"/>
-      <c r="E11" s="280"/>
-      <c r="F11" s="280"/>
-      <c r="G11" s="280"/>
-      <c r="H11" s="280"/>
-      <c r="I11" s="280"/>
-      <c r="J11" s="280"/>
-      <c r="K11" s="280"/>
-      <c r="L11" s="280"/>
-      <c r="M11" s="280"/>
-      <c r="N11" s="280"/>
-      <c r="O11" s="281"/>
-      <c r="P11" s="279" t="s">
+      <c r="C11" s="279"/>
+      <c r="D11" s="279"/>
+      <c r="E11" s="279"/>
+      <c r="F11" s="279"/>
+      <c r="G11" s="279"/>
+      <c r="H11" s="279"/>
+      <c r="I11" s="279"/>
+      <c r="J11" s="279"/>
+      <c r="K11" s="279"/>
+      <c r="L11" s="279"/>
+      <c r="M11" s="279"/>
+      <c r="N11" s="279"/>
+      <c r="O11" s="280"/>
+      <c r="P11" s="278" t="s">
         <v>62</v>
       </c>
-      <c r="Q11" s="280"/>
-      <c r="R11" s="280"/>
-      <c r="S11" s="280"/>
-      <c r="T11" s="280"/>
-      <c r="U11" s="280"/>
-      <c r="V11" s="281"/>
+      <c r="Q11" s="279"/>
+      <c r="R11" s="279"/>
+      <c r="S11" s="279"/>
+      <c r="T11" s="279"/>
+      <c r="U11" s="279"/>
+      <c r="V11" s="280"/>
     </row>
     <row r="12" spans="2:26" ht="14">
       <c r="B12" s="44" t="s">
@@ -13322,19 +13445,19 @@
       <c r="B30" s="12"/>
     </row>
     <row r="31" spans="2:24" s="61" customFormat="1" ht="14">
-      <c r="B31" s="279" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" s="280"/>
-      <c r="D31" s="280"/>
-      <c r="E31" s="280"/>
-      <c r="F31" s="280"/>
-      <c r="G31" s="280"/>
-      <c r="H31" s="280"/>
-      <c r="I31" s="280"/>
-      <c r="J31" s="280"/>
-      <c r="K31" s="280"/>
-      <c r="L31" s="281"/>
+      <c r="B31" s="278" t="s">
+        <v>0</v>
+      </c>
+      <c r="C31" s="279"/>
+      <c r="D31" s="279"/>
+      <c r="E31" s="279"/>
+      <c r="F31" s="279"/>
+      <c r="G31" s="279"/>
+      <c r="H31" s="279"/>
+      <c r="I31" s="279"/>
+      <c r="J31" s="279"/>
+      <c r="K31" s="279"/>
+      <c r="L31" s="280"/>
       <c r="M31" s="12"/>
       <c r="O31" s="12"/>
       <c r="P31" s="12"/>
@@ -14190,20 +14313,20 @@
       <c r="M50" s="64"/>
     </row>
     <row r="51" spans="2:20" s="61" customFormat="1" ht="14">
-      <c r="B51" s="279" t="s">
+      <c r="B51" s="278" t="s">
         <v>36</v>
       </c>
-      <c r="C51" s="280"/>
-      <c r="D51" s="280"/>
-      <c r="E51" s="280"/>
-      <c r="F51" s="280"/>
-      <c r="G51" s="280"/>
-      <c r="H51" s="280"/>
-      <c r="I51" s="280"/>
-      <c r="J51" s="280"/>
-      <c r="K51" s="280"/>
-      <c r="L51" s="280"/>
-      <c r="M51" s="281"/>
+      <c r="C51" s="279"/>
+      <c r="D51" s="279"/>
+      <c r="E51" s="279"/>
+      <c r="F51" s="279"/>
+      <c r="G51" s="279"/>
+      <c r="H51" s="279"/>
+      <c r="I51" s="279"/>
+      <c r="J51" s="279"/>
+      <c r="K51" s="279"/>
+      <c r="L51" s="279"/>
+      <c r="M51" s="280"/>
       <c r="O51" s="12"/>
     </row>
     <row r="52" spans="2:20" s="61" customFormat="1" ht="14">
@@ -15147,13 +15270,13 @@
       <c r="P71" s="15"/>
     </row>
     <row r="72" spans="2:25" ht="14">
-      <c r="B72" s="279" t="s">
+      <c r="B72" s="278" t="s">
         <v>58</v>
       </c>
-      <c r="C72" s="280"/>
-      <c r="D72" s="280"/>
-      <c r="E72" s="280"/>
-      <c r="F72" s="280"/>
+      <c r="C72" s="279"/>
+      <c r="D72" s="279"/>
+      <c r="E72" s="279"/>
+      <c r="F72" s="279"/>
       <c r="G72" s="45"/>
       <c r="K72" s="49"/>
     </row>
@@ -15474,13 +15597,13 @@
       <c r="K82" s="48"/>
     </row>
     <row r="83" spans="2:21" ht="14">
-      <c r="B83" s="279" t="s">
+      <c r="B83" s="278" t="s">
         <v>55</v>
       </c>
-      <c r="C83" s="280"/>
-      <c r="D83" s="280"/>
-      <c r="E83" s="280"/>
-      <c r="F83" s="280"/>
+      <c r="C83" s="279"/>
+      <c r="D83" s="279"/>
+      <c r="E83" s="279"/>
+      <c r="F83" s="279"/>
       <c r="G83" s="47"/>
       <c r="H83" s="47"/>
       <c r="I83" s="46" t="s">
@@ -15787,11 +15910,11 @@
       <c r="P93" s="15"/>
     </row>
     <row r="94" spans="2:21" ht="14">
-      <c r="B94" s="282" t="s">
+      <c r="B94" s="281" t="s">
         <v>47</v>
       </c>
-      <c r="C94" s="283"/>
-      <c r="D94" s="284"/>
+      <c r="C94" s="282"/>
+      <c r="D94" s="283"/>
       <c r="E94" s="23"/>
       <c r="F94" s="15"/>
       <c r="G94" s="22"/>
@@ -16071,11 +16194,11 @@
       <c r="A3" s="129" t="s">
         <v>160</v>
       </c>
-      <c r="B3" s="296" t="s">
+      <c r="B3" s="295" t="s">
         <v>159</v>
       </c>
-      <c r="C3" s="296"/>
-      <c r="D3" s="296"/>
+      <c r="C3" s="295"/>
+      <c r="D3" s="295"/>
       <c r="E3" s="129" t="s">
         <v>158</v>
       </c>
@@ -16266,17 +16389,17 @@
       </c>
     </row>
     <row r="27" spans="1:9">
-      <c r="A27" s="297" t="s">
+      <c r="A27" s="296" t="s">
         <v>133</v>
       </c>
-      <c r="B27" s="297"/>
-      <c r="C27" s="297"/>
-      <c r="D27" s="297"/>
-      <c r="E27" s="297"/>
-      <c r="F27" s="297"/>
-      <c r="G27" s="297"/>
-      <c r="H27" s="297"/>
-      <c r="I27" s="297"/>
+      <c r="B27" s="296"/>
+      <c r="C27" s="296"/>
+      <c r="D27" s="296"/>
+      <c r="E27" s="296"/>
+      <c r="F27" s="296"/>
+      <c r="G27" s="296"/>
+      <c r="H27" s="296"/>
+      <c r="I27" s="296"/>
     </row>
     <row r="28" spans="1:9" s="125" customFormat="1">
       <c r="A28" s="124"/>
@@ -36058,7 +36181,7 @@
       <c r="B1" s="217" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="278" t="s">
+      <c r="C1" s="277" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="220" t="s">
@@ -37980,10 +38103,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO66"/>
+  <dimension ref="A1:AO57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S34" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="U53" sqref="U53"/>
+    <sheetView tabSelected="1" topLeftCell="V8" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="AG46" sqref="AG46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -38009,12 +38132,16 @@
     <col min="19" max="19" width="10.6640625" customWidth="1"/>
     <col min="20" max="20" width="5.6640625" customWidth="1"/>
     <col min="21" max="21" width="24.83203125" customWidth="1"/>
-    <col min="22" max="22" width="21.1640625" customWidth="1"/>
+    <col min="22" max="22" width="12.5" customWidth="1"/>
     <col min="23" max="23" width="11.33203125" customWidth="1"/>
     <col min="25" max="25" width="14.33203125" customWidth="1"/>
     <col min="26" max="26" width="15.6640625" customWidth="1"/>
     <col min="27" max="27" width="21.83203125" customWidth="1"/>
     <col min="28" max="28" width="21.5" customWidth="1"/>
+    <col min="29" max="29" width="15.6640625" customWidth="1"/>
+    <col min="30" max="30" width="13.6640625" customWidth="1"/>
+    <col min="31" max="31" width="15" customWidth="1"/>
+    <col min="32" max="32" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -38210,7 +38337,7 @@
       <c r="R5" s="7"/>
       <c r="S5" s="7"/>
       <c r="T5" s="7"/>
-      <c r="U5" s="285" t="s">
+      <c r="U5" s="284" t="s">
         <v>270</v>
       </c>
       <c r="V5" s="173" t="s">
@@ -38243,7 +38370,7 @@
         <v>306</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="298" t="s">
+      <c r="C6" s="297" t="s">
         <v>308</v>
       </c>
       <c r="D6" s="7"/>
@@ -38277,7 +38404,7 @@
         <v>284</v>
       </c>
       <c r="T6" s="7"/>
-      <c r="U6" s="285"/>
+      <c r="U6" s="284"/>
       <c r="V6" s="173" t="s">
         <v>70</v>
       </c>
@@ -38346,7 +38473,7 @@
       <c r="T7" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="U7" s="285"/>
+      <c r="U7" s="284"/>
       <c r="V7" s="173" t="s">
         <v>242</v>
       </c>
@@ -38405,7 +38532,7 @@
       <c r="R8" s="162"/>
       <c r="S8" s="162"/>
       <c r="T8" s="7"/>
-      <c r="U8" s="285"/>
+      <c r="U8" s="284"/>
       <c r="V8" s="173" t="s">
         <v>240</v>
       </c>
@@ -38462,7 +38589,7 @@
       <c r="R9" s="7"/>
       <c r="S9" s="7"/>
       <c r="T9" s="7"/>
-      <c r="U9" s="285"/>
+      <c r="U9" s="284"/>
       <c r="V9" s="173" t="s">
         <v>239</v>
       </c>
@@ -38515,7 +38642,7 @@
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
       <c r="T10" s="7"/>
-      <c r="U10" s="285"/>
+      <c r="U10" s="284"/>
       <c r="V10" s="173" t="s">
         <v>238</v>
       </c>
@@ -38568,7 +38695,7 @@
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
       <c r="T11" s="7"/>
-      <c r="U11" s="285"/>
+      <c r="U11" s="284"/>
       <c r="V11" s="173" t="s">
         <v>241</v>
       </c>
@@ -38693,7 +38820,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
       <c r="L14" s="7"/>
-      <c r="M14" s="287" t="s">
+      <c r="M14" s="286" t="s">
         <v>288</v>
       </c>
       <c r="N14" s="7"/>
@@ -38706,10 +38833,10 @@
       <c r="U14" s="270" t="s">
         <v>69</v>
       </c>
-      <c r="V14" s="299"/>
-      <c r="W14" s="301"/>
-      <c r="X14" s="299"/>
-      <c r="Y14" s="303"/>
+      <c r="V14" s="298"/>
+      <c r="W14" s="300"/>
+      <c r="X14" s="298"/>
+      <c r="Y14" s="302"/>
       <c r="Z14" s="7"/>
       <c r="AA14" s="7"/>
       <c r="AB14" s="7"/>
@@ -38730,7 +38857,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
       <c r="L15" s="7"/>
-      <c r="M15" s="288"/>
+      <c r="M15" s="287"/>
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
@@ -38741,10 +38868,10 @@
       <c r="U15" s="261" t="s">
         <v>70</v>
       </c>
-      <c r="V15" s="300"/>
-      <c r="W15" s="301"/>
-      <c r="X15" s="301"/>
-      <c r="Y15" s="299"/>
+      <c r="V15" s="299"/>
+      <c r="W15" s="300"/>
+      <c r="X15" s="300"/>
+      <c r="Y15" s="298"/>
       <c r="Z15" s="7"/>
       <c r="AA15" s="7"/>
       <c r="AB15" s="7"/>
@@ -38765,7 +38892,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
       <c r="L16" s="7"/>
-      <c r="M16" s="288"/>
+      <c r="M16" s="287"/>
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
@@ -38776,14 +38903,14 @@
       <c r="U16" s="261" t="s">
         <v>242</v>
       </c>
-      <c r="V16" s="305" t="s">
+      <c r="V16" s="304" t="s">
         <v>291</v>
       </c>
-      <c r="W16" s="305" t="s">
+      <c r="W16" s="304" t="s">
         <v>291</v>
       </c>
-      <c r="X16" s="299"/>
-      <c r="Y16" s="299"/>
+      <c r="X16" s="298"/>
+      <c r="Y16" s="298"/>
       <c r="Z16" s="7"/>
       <c r="AA16" s="7"/>
       <c r="AB16" s="7"/>
@@ -38804,7 +38931,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
       <c r="L17" s="7"/>
-      <c r="M17" s="288"/>
+      <c r="M17" s="287"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
@@ -38815,14 +38942,14 @@
       <c r="U17" s="261" t="s">
         <v>240</v>
       </c>
-      <c r="V17" s="305" t="s">
+      <c r="V17" s="304" t="s">
         <v>291</v>
       </c>
-      <c r="W17" s="305" t="s">
+      <c r="W17" s="304" t="s">
         <v>291</v>
       </c>
-      <c r="X17" s="299"/>
-      <c r="Y17" s="302"/>
+      <c r="X17" s="298"/>
+      <c r="Y17" s="301"/>
       <c r="Z17" s="7"/>
       <c r="AA17" s="7"/>
       <c r="AB17" s="7"/>
@@ -38843,7 +38970,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
       <c r="L18" s="7"/>
-      <c r="M18" s="288"/>
+      <c r="M18" s="287"/>
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
@@ -38854,14 +38981,14 @@
       <c r="U18" s="261" t="s">
         <v>239</v>
       </c>
-      <c r="V18" s="305" t="s">
+      <c r="V18" s="304" t="s">
         <v>291</v>
       </c>
-      <c r="W18" s="305" t="s">
+      <c r="W18" s="304" t="s">
         <v>291</v>
       </c>
-      <c r="X18" s="302"/>
-      <c r="Y18" s="302"/>
+      <c r="X18" s="301"/>
+      <c r="Y18" s="301"/>
       <c r="Z18" s="7"/>
       <c r="AA18" s="7"/>
       <c r="AB18" s="7"/>
@@ -38882,7 +39009,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
       <c r="L19" s="7"/>
-      <c r="M19" s="288"/>
+      <c r="M19" s="287"/>
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
@@ -38893,10 +39020,10 @@
       <c r="U19" s="261" t="s">
         <v>238</v>
       </c>
-      <c r="V19" s="299"/>
-      <c r="W19" s="299"/>
-      <c r="X19" s="299"/>
-      <c r="Y19" s="299"/>
+      <c r="V19" s="298"/>
+      <c r="W19" s="298"/>
+      <c r="X19" s="298"/>
+      <c r="Y19" s="298"/>
       <c r="Z19" s="191"/>
       <c r="AA19" s="191"/>
       <c r="AB19" s="7"/>
@@ -38915,7 +39042,7 @@
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
       <c r="L20" s="10"/>
-      <c r="M20" s="289"/>
+      <c r="M20" s="288"/>
       <c r="N20" s="10"/>
       <c r="O20" s="10"/>
       <c r="P20" s="10"/>
@@ -38926,14 +39053,14 @@
       <c r="U20" s="261" t="s">
         <v>241</v>
       </c>
-      <c r="V20" s="305" t="s">
+      <c r="V20" s="304" t="s">
         <v>291</v>
       </c>
-      <c r="W20" s="305" t="s">
+      <c r="W20" s="304" t="s">
         <v>291</v>
       </c>
-      <c r="X20" s="301"/>
-      <c r="Y20" s="304"/>
+      <c r="X20" s="300"/>
+      <c r="Y20" s="303"/>
       <c r="Z20" s="10"/>
       <c r="AA20" s="10"/>
       <c r="AB20" s="10"/>
@@ -39082,7 +39209,7 @@
       <c r="R23" s="167"/>
       <c r="S23" s="167"/>
       <c r="T23" s="7"/>
-      <c r="U23" s="285" t="s">
+      <c r="U23" s="284" t="s">
         <v>271</v>
       </c>
       <c r="V23" s="173" t="s">
@@ -39133,7 +39260,7 @@
       <c r="R24" s="7"/>
       <c r="S24" s="7"/>
       <c r="T24" s="7"/>
-      <c r="U24" s="285"/>
+      <c r="U24" s="284"/>
       <c r="V24" s="173" t="s">
         <v>70</v>
       </c>
@@ -39196,7 +39323,7 @@
       <c r="R25" s="7"/>
       <c r="S25" s="7"/>
       <c r="T25" s="7"/>
-      <c r="U25" s="285"/>
+      <c r="U25" s="284"/>
       <c r="V25" s="173" t="s">
         <v>242</v>
       </c>
@@ -39261,7 +39388,7 @@
         <v>284</v>
       </c>
       <c r="T26" s="7"/>
-      <c r="U26" s="285"/>
+      <c r="U26" s="284"/>
       <c r="V26" s="173" t="s">
         <v>240</v>
       </c>
@@ -39330,7 +39457,7 @@
       <c r="T27" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="U27" s="285"/>
+      <c r="U27" s="284"/>
       <c r="V27" s="173" t="s">
         <v>239</v>
       </c>
@@ -39389,7 +39516,7 @@
       <c r="R28" s="162"/>
       <c r="S28" s="162"/>
       <c r="T28" s="7"/>
-      <c r="U28" s="285"/>
+      <c r="U28" s="284"/>
       <c r="V28" s="173" t="s">
         <v>238</v>
       </c>
@@ -39444,7 +39571,7 @@
       <c r="R29" s="7"/>
       <c r="S29" s="7"/>
       <c r="T29" s="7"/>
-      <c r="U29" s="286"/>
+      <c r="U29" s="285"/>
       <c r="V29" s="180" t="s">
         <v>241</v>
       </c>
@@ -39531,24 +39658,51 @@
       <c r="S31" s="7"/>
       <c r="T31" s="7"/>
       <c r="U31" s="7"/>
-      <c r="V31" s="167" t="s">
+      <c r="V31" s="158" t="s">
         <v>190</v>
       </c>
-      <c r="W31" s="167" t="s">
+      <c r="W31" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="X31" s="167" t="s">
+      <c r="X31" s="158" t="s">
         <v>10</v>
       </c>
-      <c r="Y31" s="167" t="s">
+      <c r="Y31" s="158" t="s">
         <v>309</v>
       </c>
-      <c r="Z31" s="167" t="s">
+      <c r="Z31" s="158" t="s">
         <v>52</v>
       </c>
-      <c r="AA31" s="7"/>
-      <c r="AB31" s="7"/>
-      <c r="AC31" s="8"/>
+      <c r="AB31" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC31" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD31" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>309</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH31" s="324" t="s">
+        <v>190</v>
+      </c>
+      <c r="AI31" s="324" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ31" s="324" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK31" s="324" t="s">
+        <v>309</v>
+      </c>
+      <c r="AL31" s="324" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="32" spans="1:41">
       <c r="A32" s="6"/>
@@ -39576,7 +39730,7 @@
       <c r="S32" s="7"/>
       <c r="T32" s="7"/>
       <c r="U32" s="7"/>
-      <c r="V32" s="167" t="s">
+      <c r="V32" s="158" t="s">
         <v>69</v>
       </c>
       <c r="W32" s="167">
@@ -39591,11 +39745,38 @@
       <c r="Z32" s="167">
         <v>9.7874443895205106E-3</v>
       </c>
-      <c r="AA32" s="7"/>
-      <c r="AB32" s="7"/>
-      <c r="AC32" s="8"/>
-    </row>
-    <row r="33" spans="1:29">
+      <c r="AB32" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC32" s="7">
+        <v>2.3858563033056299</v>
+      </c>
+      <c r="AD32" s="8">
+        <v>1.95266424480807</v>
+      </c>
+      <c r="AE32">
+        <v>2.1643015060783899</v>
+      </c>
+      <c r="AF32">
+        <v>9.7874443895205106E-3</v>
+      </c>
+      <c r="AH32" s="324" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI32" s="323">
+        <v>2.3885325302302598</v>
+      </c>
+      <c r="AJ32" s="323">
+        <v>1.95636663916208</v>
+      </c>
+      <c r="AK32" s="323">
+        <v>2.1667292138810601</v>
+      </c>
+      <c r="AL32" s="323">
+        <v>9.7984230147471207E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38">
       <c r="A33" s="6"/>
       <c r="B33" s="7"/>
       <c r="C33" s="183" t="s">
@@ -39619,7 +39800,7 @@
       <c r="S33" s="7"/>
       <c r="T33" s="7"/>
       <c r="U33" s="7"/>
-      <c r="V33" s="167" t="s">
+      <c r="V33" s="158" t="s">
         <v>70</v>
       </c>
       <c r="W33" s="167">
@@ -39634,11 +39815,38 @@
       <c r="Z33" s="167">
         <v>5.9855072463768097E-3</v>
       </c>
-      <c r="AA33" s="7"/>
-      <c r="AB33" s="7"/>
-      <c r="AC33" s="8"/>
-    </row>
-    <row r="34" spans="1:29">
+      <c r="AB33" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC33" s="7">
+        <v>3.2401656314699698</v>
+      </c>
+      <c r="AD33" s="8">
+        <v>2.7638593398168601</v>
+      </c>
+      <c r="AE33">
+        <v>1.2898765963387899</v>
+      </c>
+      <c r="AF33">
+        <v>5.9855072463768097E-3</v>
+      </c>
+      <c r="AH33" s="324" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI33" s="323">
+        <v>3.3121693121693099</v>
+      </c>
+      <c r="AJ33" s="323">
+        <v>2.8252784362572299</v>
+      </c>
+      <c r="AK33" s="323">
+        <v>1.3185405207018801</v>
+      </c>
+      <c r="AL33" s="323">
+        <v>6.1185185185185101E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38">
       <c r="A34" s="189"/>
       <c r="B34" s="163"/>
       <c r="C34" s="183" t="s">
@@ -39662,7 +39870,7 @@
       <c r="S34" s="7"/>
       <c r="T34" s="7"/>
       <c r="U34" s="7"/>
-      <c r="V34" s="167" t="s">
+      <c r="V34" s="158" t="s">
         <v>242</v>
       </c>
       <c r="W34" s="167">
@@ -39677,11 +39885,38 @@
       <c r="Z34" s="167">
         <v>3.3147899235752597E-4</v>
       </c>
-      <c r="AA34" s="7"/>
-      <c r="AB34" s="7"/>
-      <c r="AC34" s="8"/>
-    </row>
-    <row r="35" spans="1:29">
+      <c r="AB34" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC34" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE34">
+        <v>1.84350377654585</v>
+      </c>
+      <c r="AF34">
+        <v>3.3147899235752597E-4</v>
+      </c>
+      <c r="AH34" s="324" t="s">
+        <v>242</v>
+      </c>
+      <c r="AI34" s="323">
+        <v>0</v>
+      </c>
+      <c r="AJ34" s="323">
+        <v>0</v>
+      </c>
+      <c r="AK34" s="323">
+        <v>1.8514670757965901</v>
+      </c>
+      <c r="AL34" s="323">
+        <v>3.3291085952123799E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38">
       <c r="A35" s="190"/>
       <c r="B35" s="164"/>
       <c r="C35" s="183" t="s">
@@ -39705,7 +39940,7 @@
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
       <c r="U35" s="7"/>
-      <c r="V35" s="167" t="s">
+      <c r="V35" s="158" t="s">
         <v>240</v>
       </c>
       <c r="W35" s="167">
@@ -39720,11 +39955,38 @@
       <c r="Z35" s="167">
         <v>6.1582299955017399E-4</v>
       </c>
-      <c r="AA35" s="7"/>
-      <c r="AB35" s="7"/>
-      <c r="AC35" s="8"/>
-    </row>
-    <row r="36" spans="1:29">
+      <c r="AB35" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC35" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE35">
+        <v>0.64579770172648099</v>
+      </c>
+      <c r="AF35">
+        <v>6.3371304496165695E-4</v>
+      </c>
+      <c r="AH35" s="324" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI35" s="323">
+        <v>0</v>
+      </c>
+      <c r="AJ35" s="323">
+        <v>0</v>
+      </c>
+      <c r="AK35" s="323">
+        <v>0.64579404667610996</v>
+      </c>
+      <c r="AL35" s="323">
+        <v>6.3370956705190596E-4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38">
       <c r="A36" s="6"/>
       <c r="B36" s="163"/>
       <c r="C36" s="165"/>
@@ -39746,7 +40008,7 @@
       <c r="S36" s="7"/>
       <c r="T36" s="7"/>
       <c r="U36" s="7"/>
-      <c r="V36" s="167" t="s">
+      <c r="V36" s="158" t="s">
         <v>239</v>
       </c>
       <c r="W36" s="167">
@@ -39761,11 +40023,38 @@
       <c r="Z36" s="167">
         <v>3.2458463001888498E-4</v>
       </c>
-      <c r="AA36" s="7"/>
-      <c r="AB36" s="7"/>
-      <c r="AC36" s="8"/>
-    </row>
-    <row r="37" spans="1:29">
+      <c r="AB36" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <v>0.85025692281988496</v>
+      </c>
+      <c r="AF36">
+        <v>4.0917324182279397E-4</v>
+      </c>
+      <c r="AH36" s="324" t="s">
+        <v>239</v>
+      </c>
+      <c r="AI36" s="323">
+        <v>0</v>
+      </c>
+      <c r="AJ36" s="323">
+        <v>0</v>
+      </c>
+      <c r="AK36" s="323">
+        <v>0.85027782418891895</v>
+      </c>
+      <c r="AL36" s="323">
+        <v>4.0918310453618101E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38">
       <c r="A37" s="189"/>
       <c r="B37" s="163"/>
       <c r="C37" s="166" t="s">
@@ -39789,7 +40078,7 @@
       <c r="S37" s="7"/>
       <c r="T37" s="191"/>
       <c r="U37" s="7"/>
-      <c r="V37" s="167" t="s">
+      <c r="V37" s="158" t="s">
         <v>238</v>
       </c>
       <c r="W37" s="167">
@@ -39804,11 +40093,38 @@
       <c r="Z37" s="167">
         <v>1.5760003508720599E-4</v>
       </c>
-      <c r="AA37" s="7"/>
-      <c r="AB37" s="7"/>
-      <c r="AC37" s="8"/>
-    </row>
-    <row r="38" spans="1:29">
+      <c r="AB37" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC37" s="7">
+        <v>1.7465631594079999E-2</v>
+      </c>
+      <c r="AD37" s="8">
+        <v>5.3264890324061197E-2</v>
+      </c>
+      <c r="AE37">
+        <v>0.25285069520812697</v>
+      </c>
+      <c r="AF37">
+        <v>1.5760003508720599E-4</v>
+      </c>
+      <c r="AH37" s="324" t="s">
+        <v>238</v>
+      </c>
+      <c r="AI37" s="323">
+        <v>1.7465631594079999E-2</v>
+      </c>
+      <c r="AJ37" s="323">
+        <v>5.3264890324061197E-2</v>
+      </c>
+      <c r="AK37" s="323">
+        <v>0.25285069520812697</v>
+      </c>
+      <c r="AL37" s="323">
+        <v>1.5760003508720599E-4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38">
       <c r="A38" s="192"/>
       <c r="B38" s="193"/>
       <c r="C38" s="199" t="s">
@@ -39832,7 +40148,7 @@
       <c r="S38" s="7"/>
       <c r="T38" s="191"/>
       <c r="U38" s="7"/>
-      <c r="V38" s="167" t="s">
+      <c r="V38" s="158" t="s">
         <v>241</v>
       </c>
       <c r="W38" s="167">
@@ -39845,124 +40161,332 @@
         <v>0.93654462976862396</v>
       </c>
       <c r="Z38" s="167">
-        <v>2.3999999999999998E-3</v>
-      </c>
-      <c r="AA38" s="7"/>
-      <c r="AB38" s="10"/>
-      <c r="AC38" s="11"/>
-    </row>
-    <row r="39" spans="1:29">
+        <v>1.6219800000000001E-3</v>
+      </c>
+      <c r="AB38" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC38" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="11">
+        <v>0</v>
+      </c>
+      <c r="AE38">
+        <v>0.93654462976862396</v>
+      </c>
+      <c r="AF38">
+        <v>1.6219780224000001E-3</v>
+      </c>
+      <c r="AH38" s="324" t="s">
+        <v>241</v>
+      </c>
+      <c r="AI38" s="323">
+        <v>0</v>
+      </c>
+      <c r="AJ38" s="323">
+        <v>0</v>
+      </c>
+      <c r="AK38" s="323">
+        <v>0.93654462976862396</v>
+      </c>
+      <c r="AL38" s="323">
+        <v>1.6219780224000001E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38">
       <c r="S39" s="163"/>
-    </row>
-    <row r="40" spans="1:29">
+      <c r="V39" s="1"/>
+    </row>
+    <row r="40" spans="1:38">
       <c r="S40" s="163"/>
-      <c r="V40" s="306" t="s">
+      <c r="V40" s="309" t="s">
         <v>190</v>
       </c>
-      <c r="W40" s="306" t="s">
+      <c r="W40" s="309" t="s">
         <v>9</v>
       </c>
-      <c r="X40" s="306" t="s">
+      <c r="X40" s="309" t="s">
         <v>10</v>
       </c>
-      <c r="Y40" s="306" t="s">
+      <c r="Y40" s="309" t="s">
         <v>309</v>
       </c>
-      <c r="Z40" s="306" t="s">
+      <c r="Z40" s="309" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="41" spans="1:29">
+      <c r="AB40" s="309" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC40" s="309" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD40" s="309" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE40" s="309" t="s">
+        <v>309</v>
+      </c>
+      <c r="AF40" s="309" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH40" s="309" t="s">
+        <v>190</v>
+      </c>
+      <c r="AI40" s="309" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ40" s="309" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK40" s="309" t="s">
+        <v>309</v>
+      </c>
+      <c r="AL40" s="309" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38">
       <c r="S41" s="163"/>
-      <c r="V41" s="306" t="s">
+      <c r="V41" s="309" t="s">
         <v>69</v>
       </c>
-      <c r="W41" s="306">
+      <c r="W41" s="305">
         <v>2.3885325302302642</v>
       </c>
-      <c r="X41" s="306">
+      <c r="X41" s="305">
         <v>1.8845229602210121</v>
       </c>
-      <c r="Y41" s="306">
+      <c r="Y41" s="305">
         <v>2.1685682812683313</v>
       </c>
-      <c r="Z41" s="306">
+      <c r="Z41" s="305">
         <v>9.7984230147471225E-3</v>
       </c>
-    </row>
-    <row r="42" spans="1:29">
+      <c r="AB41" s="309" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC41" s="305">
+        <v>2.3885325302302642</v>
+      </c>
+      <c r="AD41" s="305">
+        <v>1.8845229602210121</v>
+      </c>
+      <c r="AE41" s="305">
+        <v>2.1685682812683313</v>
+      </c>
+      <c r="AF41" s="305">
+        <v>9.7984230147471225E-3</v>
+      </c>
+      <c r="AH41" s="309" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI41" s="305">
+        <v>2.3885325302302642</v>
+      </c>
+      <c r="AJ41" s="305">
+        <v>1.8845229602210121</v>
+      </c>
+      <c r="AK41" s="305">
+        <v>2.1685682812683313</v>
+      </c>
+      <c r="AL41" s="305">
+        <v>9.7984230147471225E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38">
       <c r="S42" s="163"/>
-      <c r="V42" s="306" t="s">
+      <c r="V42" s="309" t="s">
         <v>70</v>
       </c>
-      <c r="W42" s="306">
+      <c r="W42" s="305">
         <v>3.3121693121693125</v>
       </c>
-      <c r="X42" s="306">
+      <c r="X42" s="305">
         <v>2.8252784362572374</v>
       </c>
-      <c r="Y42" s="306">
+      <c r="Y42" s="305">
         <v>1.3189810859595519</v>
       </c>
-      <c r="Z42" s="306">
+      <c r="Z42" s="305">
         <v>6.1185185185185197E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:29">
+      <c r="AB42" s="309" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC42" s="305">
+        <v>3.3121693121693125</v>
+      </c>
+      <c r="AD42" s="305">
+        <v>2.8252784362572374</v>
+      </c>
+      <c r="AE42" s="305">
+        <v>1.3189810859595519</v>
+      </c>
+      <c r="AF42" s="305">
+        <v>6.1185185185185197E-3</v>
+      </c>
+      <c r="AH42" s="309" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI42" s="305">
+        <v>3.3121693121693125</v>
+      </c>
+      <c r="AJ42" s="305">
+        <v>2.8252784362572374</v>
+      </c>
+      <c r="AK42" s="305">
+        <v>1.3189810859595519</v>
+      </c>
+      <c r="AL42" s="305">
+        <v>6.1185185185185197E-3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38">
       <c r="S43" s="163"/>
-      <c r="V43" s="306" t="s">
+      <c r="V43" s="309" t="s">
         <v>242</v>
       </c>
-      <c r="W43" s="306">
-        <v>0</v>
-      </c>
-      <c r="X43" s="306">
-        <v>0</v>
-      </c>
-      <c r="Y43" s="306">
+      <c r="W43" s="305">
+        <v>0</v>
+      </c>
+      <c r="X43" s="305">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="305">
         <v>1.8559378643921964</v>
       </c>
-      <c r="Z43" s="306">
+      <c r="Z43" s="305">
         <v>3.3291086713062973E-4</v>
       </c>
-    </row>
-    <row r="44" spans="1:29">
+      <c r="AB43" s="309" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC43" s="305">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="305">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="305">
+        <v>1.8559378643921964</v>
+      </c>
+      <c r="AF43" s="305">
+        <v>3.3291086713062973E-4</v>
+      </c>
+      <c r="AH43" s="309" t="s">
+        <v>242</v>
+      </c>
+      <c r="AI43" s="305">
+        <v>0</v>
+      </c>
+      <c r="AJ43" s="305">
+        <v>0</v>
+      </c>
+      <c r="AK43" s="305">
+        <v>1.8559378643921964</v>
+      </c>
+      <c r="AL43" s="305">
+        <v>3.3291086713062973E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38">
       <c r="S44" s="163"/>
-      <c r="V44" s="306" t="s">
+      <c r="V44" s="309" t="s">
         <v>240</v>
       </c>
-      <c r="W44" s="306">
-        <v>0</v>
-      </c>
-      <c r="X44" s="306">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="306">
+      <c r="W44" s="305">
+        <v>0</v>
+      </c>
+      <c r="X44" s="305">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="305">
         <v>0.65412174624550123</v>
       </c>
-      <c r="Z44" s="306">
+      <c r="Z44" s="305">
         <v>6.3371300996879288E-4</v>
       </c>
-    </row>
-    <row r="45" spans="1:29">
+      <c r="AB44" s="309" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC44" s="305">
+        <v>0</v>
+      </c>
+      <c r="AD44" s="305">
+        <v>0</v>
+      </c>
+      <c r="AE44" s="305">
+        <v>0.65412174624550123</v>
+      </c>
+      <c r="AF44" s="305">
+        <v>6.3371300996879288E-4</v>
+      </c>
+      <c r="AH44" s="309" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI44" s="305">
+        <v>0</v>
+      </c>
+      <c r="AJ44" s="305">
+        <v>0</v>
+      </c>
+      <c r="AK44" s="305">
+        <v>0.65412174624550123</v>
+      </c>
+      <c r="AL44" s="305">
+        <v>6.3371300996879288E-4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38">
       <c r="S45" s="163"/>
-      <c r="V45" s="306" t="s">
+      <c r="V45" s="309" t="s">
         <v>239</v>
       </c>
-      <c r="W45" s="306">
-        <v>0</v>
-      </c>
-      <c r="X45" s="306">
-        <v>0</v>
-      </c>
-      <c r="Y45" s="306">
+      <c r="W45" s="305">
+        <v>0</v>
+      </c>
+      <c r="X45" s="305">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="305">
         <v>0.85464548272482521</v>
       </c>
-      <c r="Z45" s="306">
+      <c r="Z45" s="305">
         <v>4.0896884727136267E-4</v>
       </c>
-    </row>
-    <row r="46" spans="1:29">
+      <c r="AB45" s="309" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC45" s="305">
+        <v>0</v>
+      </c>
+      <c r="AD45" s="305">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="305">
+        <v>0.85464548272482521</v>
+      </c>
+      <c r="AF45" s="305">
+        <v>4.0896884727136267E-4</v>
+      </c>
+      <c r="AH45" s="309" t="s">
+        <v>239</v>
+      </c>
+      <c r="AI45" s="305">
+        <v>0</v>
+      </c>
+      <c r="AJ45" s="305">
+        <v>0</v>
+      </c>
+      <c r="AK45" s="305">
+        <v>0.85464548272482521</v>
+      </c>
+      <c r="AL45" s="305">
+        <v>4.0896884727136267E-4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38">
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
       <c r="J46" s="2"/>
@@ -39973,23 +40497,53 @@
       <c r="O46" s="2"/>
       <c r="P46" s="2"/>
       <c r="S46" s="163"/>
-      <c r="V46" s="306" t="s">
+      <c r="V46" s="309" t="s">
         <v>238</v>
       </c>
-      <c r="W46" s="306">
+      <c r="W46" s="305">
         <v>1.7469371020292866E-2</v>
       </c>
-      <c r="X46" s="306">
+      <c r="X46" s="305">
         <v>5.328404484933285E-2</v>
       </c>
-      <c r="Y46" s="306">
+      <c r="Y46" s="305">
         <v>0.25324815656620991</v>
       </c>
-      <c r="Z46" s="306">
+      <c r="Z46" s="305">
         <v>1.5761936755060593E-4</v>
       </c>
-    </row>
-    <row r="47" spans="1:29">
+      <c r="AB46" s="309" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC46" s="305">
+        <v>1.7469371020292866E-2</v>
+      </c>
+      <c r="AD46" s="305">
+        <v>5.328404484933285E-2</v>
+      </c>
+      <c r="AE46" s="305">
+        <v>0.25324815656620991</v>
+      </c>
+      <c r="AF46" s="305">
+        <v>1.5761936755060593E-4</v>
+      </c>
+      <c r="AH46" s="309" t="s">
+        <v>238</v>
+      </c>
+      <c r="AI46" s="305">
+        <v>1.7469371020292866E-2</v>
+      </c>
+      <c r="AJ46" s="305">
+        <v>5.328404484933285E-2</v>
+      </c>
+      <c r="AK46" s="305">
+        <v>0.25324815656620991</v>
+      </c>
+      <c r="AL46" s="305">
+        <v>1.5761936755060593E-4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38">
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
       <c r="J47" s="2"/>
@@ -40000,23 +40554,53 @@
       <c r="O47" s="2"/>
       <c r="P47" s="2"/>
       <c r="S47" s="163"/>
-      <c r="V47" s="306" t="s">
+      <c r="V47" s="309" t="s">
         <v>241</v>
       </c>
-      <c r="W47" s="306">
-        <v>0</v>
-      </c>
-      <c r="X47" s="306">
-        <v>0</v>
-      </c>
-      <c r="Y47" s="306">
+      <c r="W47" s="305">
+        <v>0</v>
+      </c>
+      <c r="X47" s="305">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="305">
         <v>0.949145345916109</v>
       </c>
-      <c r="Z47" s="306">
+      <c r="Z47" s="305">
         <v>1.6310469912058185E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:29">
+      <c r="AB47" s="309" t="s">
+        <v>241</v>
+      </c>
+      <c r="AC47" s="305">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="305">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="305">
+        <v>0.949145345916109</v>
+      </c>
+      <c r="AF47" s="305">
+        <v>1.6310469912058185E-3</v>
+      </c>
+      <c r="AH47" s="309" t="s">
+        <v>241</v>
+      </c>
+      <c r="AI47" s="305">
+        <v>0</v>
+      </c>
+      <c r="AJ47" s="305">
+        <v>0</v>
+      </c>
+      <c r="AK47" s="305">
+        <v>0.949145345916109</v>
+      </c>
+      <c r="AL47" s="305">
+        <v>1.6310469912058185E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38">
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2"/>
@@ -40027,8 +40611,9 @@
       <c r="O48" s="2"/>
       <c r="P48" s="2"/>
       <c r="S48" s="163"/>
-    </row>
-    <row r="49" spans="8:26">
+      <c r="V48" s="1"/>
+    </row>
+    <row r="49" spans="8:38">
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2"/>
@@ -40039,23 +40624,53 @@
       <c r="O49" s="2"/>
       <c r="P49" s="2"/>
       <c r="S49" s="163"/>
-      <c r="V49" s="307" t="s">
+      <c r="V49" s="310" t="s">
         <v>190</v>
       </c>
-      <c r="W49" s="307" t="s">
+      <c r="W49" s="310" t="s">
         <v>9</v>
       </c>
-      <c r="X49" s="307" t="s">
+      <c r="X49" s="310" t="s">
         <v>10</v>
       </c>
-      <c r="Y49" s="307" t="s">
+      <c r="Y49" s="310" t="s">
         <v>309</v>
       </c>
-      <c r="Z49" s="307" t="s">
+      <c r="Z49" s="310" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="50" spans="8:26">
+      <c r="AB49" s="309" t="s">
+        <v>190</v>
+      </c>
+      <c r="AC49" s="309" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD49" s="309" t="s">
+        <v>10</v>
+      </c>
+      <c r="AE49" s="309" t="s">
+        <v>309</v>
+      </c>
+      <c r="AF49" s="309" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH49" s="321" t="s">
+        <v>190</v>
+      </c>
+      <c r="AI49" s="321" t="s">
+        <v>9</v>
+      </c>
+      <c r="AJ49" s="321" t="s">
+        <v>10</v>
+      </c>
+      <c r="AK49" s="321" t="s">
+        <v>309</v>
+      </c>
+      <c r="AL49" s="321" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="50" spans="8:38">
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -40066,27 +40681,65 @@
       <c r="O50" s="2"/>
       <c r="P50" s="2"/>
       <c r="S50" s="163"/>
-      <c r="V50" s="307" t="s">
+      <c r="V50" s="310" t="s">
         <v>69</v>
       </c>
-      <c r="W50" s="308">
+      <c r="W50" s="306">
         <f xml:space="preserve"> W32/W41</f>
         <v>0.99887955182072552</v>
       </c>
-      <c r="X50" s="308">
-        <f xml:space="preserve"> X32/X41</f>
-        <v>1.0361583732463873</v>
-      </c>
-      <c r="Y50" s="308">
+      <c r="X50" s="307">
+        <f>X41/ X32</f>
+        <v>0.96510342995820275</v>
+      </c>
+      <c r="Y50" s="306">
         <f xml:space="preserve"> Y32/Y41</f>
         <v>0.99803244600283192</v>
       </c>
-      <c r="Z50" s="308">
+      <c r="Z50" s="306">
         <f xml:space="preserve"> Z32/Z41</f>
         <v>0.99887955182072785</v>
       </c>
-    </row>
-    <row r="51" spans="8:26">
+      <c r="AB50" s="309" t="s">
+        <v>69</v>
+      </c>
+      <c r="AC50" s="320">
+        <f>AC32/AC41</f>
+        <v>0.99887955182072552</v>
+      </c>
+      <c r="AD50" s="320">
+        <f>AD32/AD41</f>
+        <v>1.0361583732463873</v>
+      </c>
+      <c r="AE50" s="320">
+        <f>AE32/AE41</f>
+        <v>0.99803244600283192</v>
+      </c>
+      <c r="AF50" s="320">
+        <f>AF32/AF41</f>
+        <v>0.99887955182072785</v>
+      </c>
+      <c r="AH50" s="321" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI50" s="322">
+        <f>AI32/AI41</f>
+        <v>0.99999999999999811</v>
+      </c>
+      <c r="AJ50" s="322">
+        <f>AJ32/AJ41</f>
+        <v>1.0381230053746027</v>
+      </c>
+      <c r="AK50" s="322">
+        <f>AK32/AK41</f>
+        <v>0.99915194397928031</v>
+      </c>
+      <c r="AL50" s="322">
+        <f>AL32/AL41</f>
+        <v>0.99999999999999978</v>
+      </c>
+    </row>
+    <row r="51" spans="8:38">
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -40097,27 +40750,65 @@
       <c r="O51" s="2"/>
       <c r="P51" s="2"/>
       <c r="S51" s="163"/>
-      <c r="V51" s="307" t="s">
+      <c r="V51" s="310" t="s">
         <v>70</v>
       </c>
-      <c r="W51" s="308">
+      <c r="W51" s="306">
         <f xml:space="preserve"> W33/W42</f>
         <v>0.97826086956521441</v>
       </c>
-      <c r="X51" s="308">
+      <c r="X51" s="306">
         <f xml:space="preserve"> X33/X42</f>
         <v>0.97826086956521641</v>
       </c>
-      <c r="Y51" s="308">
+      <c r="Y51" s="306">
         <f xml:space="preserve"> Y33/Y42</f>
         <v>0.97793411146636078</v>
       </c>
-      <c r="Z51" s="308">
+      <c r="Z51" s="306">
         <f xml:space="preserve"> Z33/Z42</f>
         <v>0.97826086956521685</v>
       </c>
-    </row>
-    <row r="52" spans="8:26">
+      <c r="AB51" s="309" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC51" s="320">
+        <f t="shared" ref="AC51:AD51" si="0">AC33/AC42</f>
+        <v>0.97826086956521441</v>
+      </c>
+      <c r="AD51" s="320">
+        <f t="shared" si="0"/>
+        <v>0.97826086956521641</v>
+      </c>
+      <c r="AE51" s="320">
+        <f t="shared" ref="AE51:AF51" si="1">AE33/AE42</f>
+        <v>0.97793411146636078</v>
+      </c>
+      <c r="AF51" s="320">
+        <f t="shared" si="1"/>
+        <v>0.97826086956521685</v>
+      </c>
+      <c r="AH51" s="321" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI51" s="322">
+        <f>AI33/AI42</f>
+        <v>0.99999999999999922</v>
+      </c>
+      <c r="AJ51" s="322">
+        <f>AJ33/AJ42</f>
+        <v>0.99999999999999734</v>
+      </c>
+      <c r="AK51" s="322">
+        <f>AK33/AK42</f>
+        <v>0.99966598061006218</v>
+      </c>
+      <c r="AL51" s="322">
+        <f>AL33/AL42</f>
+        <v>0.99999999999999845</v>
+      </c>
+    </row>
+    <row r="52" spans="8:38">
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -40127,21 +40818,47 @@
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
       <c r="P52" s="2"/>
-      <c r="V52" s="307" t="s">
+      <c r="V52" s="310" t="s">
         <v>242</v>
       </c>
-      <c r="W52" s="308"/>
-      <c r="X52" s="308"/>
-      <c r="Y52" s="308">
+      <c r="W52" s="306"/>
+      <c r="X52" s="306"/>
+      <c r="Y52" s="306">
         <f xml:space="preserve"> Y34/Y43</f>
         <v>0.99330037492908285</v>
       </c>
-      <c r="Z52" s="308">
+      <c r="Z52" s="306">
         <f xml:space="preserve"> Z34/Z43</f>
         <v>0.99569892450359121</v>
       </c>
-    </row>
-    <row r="53" spans="8:26">
+      <c r="AB52" s="309" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC52" s="320"/>
+      <c r="AD52" s="320"/>
+      <c r="AE52" s="320">
+        <f t="shared" ref="AE52:AF52" si="2">AE34/AE43</f>
+        <v>0.99330037492908285</v>
+      </c>
+      <c r="AF52" s="320">
+        <f t="shared" si="2"/>
+        <v>0.99569892450359121</v>
+      </c>
+      <c r="AH52" s="321" t="s">
+        <v>242</v>
+      </c>
+      <c r="AI52" s="322"/>
+      <c r="AJ52" s="322"/>
+      <c r="AK52" s="322">
+        <f>AK34/AK43</f>
+        <v>0.99759108929162854</v>
+      </c>
+      <c r="AL52" s="322">
+        <f>AL34/AL43</f>
+        <v>0.99999997714285571</v>
+      </c>
+    </row>
+    <row r="53" spans="8:38">
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -40151,21 +40868,47 @@
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
       <c r="P53" s="2"/>
-      <c r="V53" s="307" t="s">
+      <c r="V53" s="310" t="s">
         <v>240</v>
       </c>
-      <c r="W53" s="308"/>
-      <c r="X53" s="308"/>
-      <c r="Y53" s="309">
+      <c r="W53" s="306"/>
+      <c r="X53" s="306"/>
+      <c r="Y53" s="307">
         <f xml:space="preserve"> Y35/Y44</f>
         <v>0.95940320565248305</v>
       </c>
-      <c r="Z53" s="308">
+      <c r="Z53" s="306">
         <f xml:space="preserve"> Z35/Z44</f>
         <v>0.97176953899131746</v>
       </c>
-    </row>
-    <row r="54" spans="8:26">
+      <c r="AB53" s="309" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC53" s="320"/>
+      <c r="AD53" s="320"/>
+      <c r="AE53" s="320">
+        <f t="shared" ref="AE53:AF53" si="3">AE35/AE44</f>
+        <v>0.98727447211960428</v>
+      </c>
+      <c r="AF53" s="320">
+        <f t="shared" si="3"/>
+        <v>1.0000000552187875</v>
+      </c>
+      <c r="AH53" s="321" t="s">
+        <v>240</v>
+      </c>
+      <c r="AI53" s="322"/>
+      <c r="AJ53" s="322"/>
+      <c r="AK53" s="322">
+        <f>AK35/AK44</f>
+        <v>0.98726888439775895</v>
+      </c>
+      <c r="AL53" s="322">
+        <f>AL35/AL44</f>
+        <v>0.99999456707242429</v>
+      </c>
+    </row>
+    <row r="54" spans="8:38">
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
@@ -40175,21 +40918,47 @@
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
       <c r="P54" s="2"/>
-      <c r="V54" s="307" t="s">
+      <c r="V54" s="310" t="s">
         <v>239</v>
       </c>
-      <c r="W54" s="308"/>
-      <c r="X54" s="308"/>
-      <c r="Y54" s="310">
+      <c r="W54" s="306"/>
+      <c r="X54" s="306"/>
+      <c r="Y54" s="308">
         <f xml:space="preserve"> Y36/Y45</f>
         <v>0.78919604679504862</v>
       </c>
-      <c r="Z54" s="310">
+      <c r="Z54" s="308">
         <f xml:space="preserve"> Z36/Z45</f>
         <v>0.79366590434579898</v>
       </c>
-    </row>
-    <row r="55" spans="8:26">
+      <c r="AB54" s="309" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC54" s="320"/>
+      <c r="AD54" s="320"/>
+      <c r="AE54" s="320">
+        <f t="shared" ref="AE54:AF54" si="4">AE36/AE45</f>
+        <v>0.99486505224254107</v>
+      </c>
+      <c r="AF54" s="320">
+        <f t="shared" si="4"/>
+        <v>1.0004997802468207</v>
+      </c>
+      <c r="AH54" s="321" t="s">
+        <v>239</v>
+      </c>
+      <c r="AI54" s="322"/>
+      <c r="AJ54" s="322"/>
+      <c r="AK54" s="322">
+        <f>AK36/AK45</f>
+        <v>0.99488950842871005</v>
+      </c>
+      <c r="AL54" s="322">
+        <f>AL36/AL45</f>
+        <v>1.0005238962973533</v>
+      </c>
+    </row>
+    <row r="55" spans="8:38">
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
       <c r="J55" s="2"/>
@@ -40199,145 +40968,107 @@
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
       <c r="P55" s="2"/>
-      <c r="V55" s="307" t="s">
+      <c r="V55" s="310" t="s">
         <v>238</v>
       </c>
-      <c r="W55" s="308">
+      <c r="W55" s="306">
         <f xml:space="preserve"> W37/W46</f>
         <v>0.9997859438551896</v>
       </c>
-      <c r="X55" s="308">
+      <c r="X55" s="306">
         <f xml:space="preserve"> X37/X46</f>
         <v>0.99964052043485407</v>
       </c>
-      <c r="Y55" s="308">
+      <c r="Y55" s="306">
         <f xml:space="preserve"> Y37/Y46</f>
         <v>0.99843054589825209</v>
       </c>
-      <c r="Z55" s="308">
+      <c r="Z55" s="306">
         <f xml:space="preserve"> Z37/Z46</f>
         <v>0.999877347157901</v>
       </c>
-    </row>
-    <row r="56" spans="8:26">
-      <c r="V56" s="307" t="s">
+      <c r="AB55" s="309" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC55" s="320">
+        <f t="shared" ref="AC55:AD55" si="5">AC37/AC46</f>
+        <v>0.9997859438551896</v>
+      </c>
+      <c r="AD55" s="320">
+        <f t="shared" si="5"/>
+        <v>0.99964052043485407</v>
+      </c>
+      <c r="AE55" s="320">
+        <f t="shared" ref="AE55:AF55" si="6">AE37/AE46</f>
+        <v>0.99843054589825209</v>
+      </c>
+      <c r="AF55" s="320">
+        <f t="shared" si="6"/>
+        <v>0.999877347157901</v>
+      </c>
+      <c r="AH55" s="321" t="s">
+        <v>238</v>
+      </c>
+      <c r="AI55" s="322">
+        <f>AI37/AI46</f>
+        <v>0.9997859438551896</v>
+      </c>
+      <c r="AJ55" s="322">
+        <f>AJ37/AJ46</f>
+        <v>0.99964052043485407</v>
+      </c>
+      <c r="AK55" s="322">
+        <f>AK37/AK46</f>
+        <v>0.99843054589825209</v>
+      </c>
+      <c r="AL55" s="322">
+        <f>AL37/AL46</f>
+        <v>0.999877347157901</v>
+      </c>
+    </row>
+    <row r="56" spans="8:38">
+      <c r="V56" s="310" t="s">
         <v>241</v>
       </c>
-      <c r="W56" s="308"/>
-      <c r="X56" s="308"/>
-      <c r="Y56" s="308">
+      <c r="W56" s="306"/>
+      <c r="X56" s="306"/>
+      <c r="Y56" s="306">
         <f xml:space="preserve"> Y38/Y47</f>
         <v>0.98672414483018622</v>
       </c>
-      <c r="Z56" s="310">
+      <c r="Z56" s="306">
         <f xml:space="preserve"> Z47/Z38</f>
-        <v>0.67960291300242448</v>
-      </c>
-    </row>
-    <row r="58" spans="8:26">
-      <c r="V58" s="266" t="s">
-        <v>289</v>
-      </c>
-      <c r="W58" s="267"/>
-      <c r="X58" s="268"/>
-      <c r="Y58" s="268"/>
-      <c r="Z58" s="269"/>
-    </row>
-    <row r="59" spans="8:26">
-      <c r="V59" s="270" t="s">
-        <v>305</v>
-      </c>
-      <c r="W59" s="271" t="s">
-        <v>261</v>
-      </c>
-      <c r="X59" s="272" t="s">
-        <v>262</v>
-      </c>
-      <c r="Y59" s="270" t="s">
-        <v>290</v>
-      </c>
-      <c r="Z59" s="261" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="60" spans="8:26">
-      <c r="V60" s="270" t="s">
-        <v>69</v>
-      </c>
-      <c r="W60" s="299"/>
-      <c r="X60" s="301"/>
-      <c r="Y60" s="299"/>
-      <c r="Z60" s="303"/>
-    </row>
-    <row r="61" spans="8:26">
-      <c r="V61" s="261" t="s">
-        <v>70</v>
-      </c>
-      <c r="W61" s="300"/>
-      <c r="X61" s="301"/>
-      <c r="Y61" s="301"/>
-      <c r="Z61" s="299"/>
-    </row>
-    <row r="62" spans="8:26">
-      <c r="V62" s="261" t="s">
-        <v>242</v>
-      </c>
-      <c r="W62" s="305" t="s">
-        <v>291</v>
-      </c>
-      <c r="X62" s="305" t="s">
-        <v>291</v>
-      </c>
-      <c r="Y62" s="299"/>
-      <c r="Z62" s="299"/>
-    </row>
-    <row r="63" spans="8:26">
-      <c r="V63" s="261" t="s">
-        <v>240</v>
-      </c>
-      <c r="W63" s="305" t="s">
-        <v>291</v>
-      </c>
-      <c r="X63" s="305" t="s">
-        <v>291</v>
-      </c>
-      <c r="Y63" s="299"/>
-      <c r="Z63" s="302"/>
-    </row>
-    <row r="64" spans="8:26">
-      <c r="V64" s="261" t="s">
-        <v>239</v>
-      </c>
-      <c r="W64" s="305" t="s">
-        <v>291</v>
-      </c>
-      <c r="X64" s="305" t="s">
-        <v>291</v>
-      </c>
-      <c r="Y64" s="302"/>
-      <c r="Z64" s="302"/>
-    </row>
-    <row r="65" spans="22:26">
-      <c r="V65" s="261" t="s">
-        <v>238</v>
-      </c>
-      <c r="W65" s="299"/>
-      <c r="X65" s="299"/>
-      <c r="Y65" s="299"/>
-      <c r="Z65" s="299"/>
-    </row>
-    <row r="66" spans="22:26">
-      <c r="V66" s="261" t="s">
+        <v>1.0055900758368281</v>
+      </c>
+      <c r="AB56" s="309" t="s">
         <v>241</v>
       </c>
-      <c r="W66" s="305" t="s">
-        <v>291</v>
-      </c>
-      <c r="X66" s="305" t="s">
-        <v>291</v>
-      </c>
-      <c r="Y66" s="301"/>
-      <c r="Z66" s="304"/>
+      <c r="AC56" s="320"/>
+      <c r="AD56" s="320"/>
+      <c r="AE56" s="320">
+        <f t="shared" ref="AE56:AF56" si="7">AE38/AE47</f>
+        <v>0.98672414483018622</v>
+      </c>
+      <c r="AF56" s="320">
+        <f t="shared" si="7"/>
+        <v>0.99443978692538226</v>
+      </c>
+      <c r="AH56" s="321" t="s">
+        <v>241</v>
+      </c>
+      <c r="AI56" s="322"/>
+      <c r="AJ56" s="322"/>
+      <c r="AK56" s="322">
+        <f>AK38/AK47</f>
+        <v>0.98672414483018622</v>
+      </c>
+      <c r="AL56" s="322">
+        <f>AL38/AL47</f>
+        <v>0.99443978692538226</v>
+      </c>
+    </row>
+    <row r="57" spans="8:38">
+      <c r="V57" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -40360,21 +41091,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X959"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0"/>
+    <sheetView topLeftCell="A11" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:I18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="73.5" style="234" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" style="234" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" style="206" customWidth="1"/>
     <col min="3" max="3" width="9.33203125" style="206" customWidth="1"/>
-    <col min="4" max="4" width="25" style="206" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" style="206" customWidth="1"/>
     <col min="5" max="6" width="8.83203125" style="206" customWidth="1"/>
     <col min="7" max="7" width="18.6640625" style="206" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5" style="206" customWidth="1"/>
-    <col min="9" max="9" width="4.5" style="206" customWidth="1"/>
+    <col min="8" max="8" width="13" style="206" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" style="206" customWidth="1"/>
     <col min="10" max="10" width="18.5" style="206" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="206" customWidth="1"/>
-    <col min="12" max="12" width="37.5" style="206" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" style="206" customWidth="1"/>
     <col min="13" max="16384" width="14.5" style="206"/>
   </cols>
   <sheetData>
@@ -40725,130 +41458,958 @@
     <row r="11" spans="1:24" ht="14">
       <c r="A11" s="220"/>
       <c r="B11" s="220"/>
+      <c r="I11" s="206" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:24" ht="14">
       <c r="A12" s="252"/>
       <c r="B12" s="252"/>
       <c r="C12" s="273"/>
+      <c r="H12" s="315" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="206">
+        <v>4.6252066014017901E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:24" ht="14">
-      <c r="A13" s="220"/>
-      <c r="B13" s="221"/>
-      <c r="C13" s="217"/>
-      <c r="H13" s="218"/>
+      <c r="B13" s="311" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="273" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="234" t="s">
+        <v>242</v>
+      </c>
+      <c r="E13" s="234" t="s">
+        <v>240</v>
+      </c>
+      <c r="F13" s="312" t="s">
+        <v>239</v>
+      </c>
+      <c r="H13" s="316" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="206">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:24" ht="14">
-      <c r="A14" s="206"/>
-      <c r="B14" s="221"/>
-      <c r="C14" s="224"/>
+      <c r="A14" s="208" t="s">
+        <v>310</v>
+      </c>
+      <c r="B14" s="221">
+        <v>1</v>
+      </c>
+      <c r="C14" s="224">
+        <v>1</v>
+      </c>
+      <c r="D14" s="206">
+        <v>0.48611111099999998</v>
+      </c>
+      <c r="E14" s="206">
+        <v>0.256410256</v>
+      </c>
+      <c r="F14" s="313">
+        <v>9.6153846000000001E-2</v>
+      </c>
+      <c r="H14" s="316" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14" s="206">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:24" ht="14">
-      <c r="A15" s="206"/>
-      <c r="B15" s="224"/>
-      <c r="F15" s="277"/>
+      <c r="A15" s="234" t="s">
+        <v>311</v>
+      </c>
+      <c r="B15" s="224">
+        <v>8</v>
+      </c>
+      <c r="D15" s="206">
+        <v>2.4</v>
+      </c>
+      <c r="E15" s="206">
+        <v>1.115384615</v>
+      </c>
+      <c r="F15" s="314">
+        <v>1.115384615</v>
+      </c>
+      <c r="H15" s="316" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="206">
+        <v>1.31617553460685E-3</v>
+      </c>
     </row>
     <row r="16" spans="1:24" ht="14">
-      <c r="F16" s="277"/>
-    </row>
-    <row r="17" spans="1:10" ht="14">
-      <c r="A17" s="252"/>
-      <c r="B17" s="252"/>
-    </row>
-    <row r="18" spans="1:10" s="208" customFormat="1" ht="14">
-      <c r="A18" s="220"/>
-      <c r="B18" s="217"/>
-      <c r="C18" s="206"/>
-      <c r="D18" s="206"/>
-      <c r="E18" s="206"/>
-      <c r="F18" s="206"/>
-    </row>
-    <row r="19" spans="1:10" s="220" customFormat="1" ht="14">
-      <c r="F19" s="206"/>
-    </row>
-    <row r="20" spans="1:10" s="220" customFormat="1" ht="14">
-      <c r="F20" s="206"/>
-    </row>
-    <row r="21" spans="1:10" ht="14"/>
-    <row r="22" spans="1:10" ht="14"/>
-    <row r="23" spans="1:10" ht="14"/>
-    <row r="24" spans="1:10" ht="14">
-      <c r="G24" s="277"/>
-      <c r="H24" s="277"/>
-      <c r="I24" s="277"/>
-      <c r="J24" s="277"/>
-    </row>
-    <row r="25" spans="1:10" ht="14">
-      <c r="G25" s="277"/>
-      <c r="H25" s="277"/>
-      <c r="I25" s="277"/>
-      <c r="J25" s="277"/>
-    </row>
-    <row r="26" spans="1:10" ht="14"/>
-    <row r="27" spans="1:10" ht="14">
-      <c r="G27" s="228"/>
-      <c r="H27" s="228"/>
-    </row>
-    <row r="28" spans="1:10" ht="14">
-      <c r="A28" s="206"/>
-    </row>
-    <row r="29" spans="1:10" ht="14">
-      <c r="A29" s="206"/>
-    </row>
-    <row r="30" spans="1:10" ht="14">
-      <c r="A30" s="206"/>
-    </row>
-    <row r="31" spans="1:10" ht="14">
-      <c r="A31" s="206"/>
-    </row>
-    <row r="32" spans="1:10" ht="14">
-      <c r="A32" s="206"/>
-    </row>
-    <row r="33" spans="1:1" ht="14">
-      <c r="A33" s="206"/>
-    </row>
-    <row r="34" spans="1:1" ht="14">
-      <c r="A34" s="206"/>
-    </row>
-    <row r="35" spans="1:1" ht="14">
-      <c r="A35" s="206"/>
-    </row>
-    <row r="36" spans="1:1" ht="14">
-      <c r="A36" s="206"/>
-    </row>
-    <row r="37" spans="1:1" ht="14">
-      <c r="A37" s="206"/>
-    </row>
-    <row r="38" spans="1:1" ht="14">
-      <c r="A38" s="206"/>
-    </row>
-    <row r="39" spans="1:1" ht="14">
-      <c r="A39" s="206"/>
-    </row>
-    <row r="40" spans="1:1" ht="14">
-      <c r="A40" s="206"/>
-    </row>
-    <row r="41" spans="1:1" ht="14">
-      <c r="A41" s="206"/>
-    </row>
-    <row r="42" spans="1:1" ht="14">
+      <c r="A16" s="234" t="s">
+        <v>75</v>
+      </c>
+      <c r="B16" s="206">
+        <v>1.25</v>
+      </c>
+      <c r="D16" s="206">
+        <v>0.91666666699999999</v>
+      </c>
+      <c r="E16" s="206">
+        <v>0.61538461499999997</v>
+      </c>
+      <c r="F16" s="314">
+        <v>0.351648352</v>
+      </c>
+      <c r="H16" s="316" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" s="206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="14">
+      <c r="A17" s="234" t="s">
+        <v>312</v>
+      </c>
+      <c r="B17" s="252">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="C17" s="206">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D17" s="206">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="E17" s="206">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F17" s="313">
+        <v>2E-3</v>
+      </c>
+      <c r="H17" s="316" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="206">
+        <v>1.7983511221945101E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" s="208" customFormat="1" ht="14">
+      <c r="A18" s="252" t="s">
+        <v>313</v>
+      </c>
+      <c r="B18" s="217">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="C18" s="206">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D18" s="206">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="E18" s="206">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F18" s="313">
+        <v>2E-3</v>
+      </c>
+      <c r="H18" s="317" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="206">
+        <v>2.6536278743300502E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" s="220" customFormat="1" ht="14">
+      <c r="A19" s="208" t="s">
+        <v>314</v>
+      </c>
+      <c r="B19" s="220">
+        <v>6.75</v>
+      </c>
+      <c r="C19" s="220">
+        <v>8</v>
+      </c>
+      <c r="D19" s="220">
+        <v>2.4</v>
+      </c>
+      <c r="E19" s="220">
+        <v>0.5</v>
+      </c>
+      <c r="F19" s="313">
+        <v>1.115</v>
+      </c>
+      <c r="H19" s="317" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" s="220" customFormat="1" ht="14">
+      <c r="A20" s="208" t="s">
+        <v>315</v>
+      </c>
+      <c r="B20" s="220">
+        <v>0.85</v>
+      </c>
+      <c r="C20" s="220">
+        <v>1.5</v>
+      </c>
+      <c r="D20" s="220">
+        <v>24</v>
+      </c>
+      <c r="E20" s="220">
+        <v>88.918999999999997</v>
+      </c>
+      <c r="F20" s="313">
+        <v>81.980999999999995</v>
+      </c>
+      <c r="H20" s="317" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="14">
+      <c r="A21" s="208" t="s">
+        <v>316</v>
+      </c>
+      <c r="B21" s="206">
+        <v>0.17</v>
+      </c>
+      <c r="C21" s="206">
+        <v>0.08</v>
+      </c>
+      <c r="D21" s="206">
+        <v>0.02</v>
+      </c>
+      <c r="E21" s="206">
+        <v>0.02</v>
+      </c>
+      <c r="F21" s="313">
+        <v>0.01</v>
+      </c>
+      <c r="H21" s="317" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" s="206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="14">
+      <c r="H22" s="319" t="s">
+        <v>309</v>
+      </c>
+      <c r="I22" s="313">
+        <v>1.03933611325332E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="14"/>
+    <row r="24" spans="1:12" ht="14">
+      <c r="A24" s="315" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="315" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" s="316" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="316" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="316" t="s">
+        <v>5</v>
+      </c>
+      <c r="F24" s="316" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="316" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="317" t="s">
+        <v>8</v>
+      </c>
+      <c r="I24" s="317" t="s">
+        <v>9</v>
+      </c>
+      <c r="J24" s="317" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="317" t="s">
+        <v>11</v>
+      </c>
+      <c r="L24" s="316" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="14">
+      <c r="A25" s="315" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="315">
+        <v>0</v>
+      </c>
+      <c r="C25" s="316">
+        <v>1.46783012340111E-2</v>
+      </c>
+      <c r="D25" s="316">
+        <v>0.18931341408459801</v>
+      </c>
+      <c r="E25" s="316">
+        <v>1.24657925026367E-4</v>
+      </c>
+      <c r="F25" s="316">
+        <v>0</v>
+      </c>
+      <c r="G25" s="316">
+        <v>5.1097755610972503E-4</v>
+      </c>
+      <c r="H25" s="317">
+        <v>6.4089412775986E-3</v>
+      </c>
+      <c r="I25" s="317">
+        <v>0.48952380952380897</v>
+      </c>
+      <c r="J25" s="317">
+        <v>0.41931877068780798</v>
+      </c>
+      <c r="K25" s="317">
+        <v>4.6347753980447402E-3</v>
+      </c>
+      <c r="L25" s="316">
+        <v>0.215671067475389</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="14">
+      <c r="A26" s="315" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="315">
+        <v>0</v>
+      </c>
+      <c r="C26" s="316">
+        <v>5.1199108407630296E-3</v>
+      </c>
+      <c r="D26" s="316">
+        <v>0.15713919424638301</v>
+      </c>
+      <c r="E26" s="316">
+        <v>0</v>
+      </c>
+      <c r="F26" s="316">
+        <v>0</v>
+      </c>
+      <c r="G26" s="316">
+        <v>2.54618703241895E-3</v>
+      </c>
+      <c r="H26" s="316">
+        <v>6.3871166797965298E-3</v>
+      </c>
+      <c r="I26" s="316">
+        <v>0.48214285714285698</v>
+      </c>
+      <c r="J26" s="316">
+        <v>0.44899725410719699</v>
+      </c>
+      <c r="K26" s="316">
+        <v>2.27810994141182E-3</v>
+      </c>
+      <c r="L26" s="316">
+        <v>0.17347051874077399</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="14">
+      <c r="A27" s="315" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="315">
+        <v>4.1483730728559501E-4</v>
+      </c>
+      <c r="C27" s="316">
+        <v>9.5665045722475896E-3</v>
+      </c>
+      <c r="D27" s="316">
+        <v>0.289592983208321</v>
+      </c>
+      <c r="E27" s="316">
+        <v>7.7495346172529499E-3</v>
+      </c>
+      <c r="F27" s="316">
+        <v>0</v>
+      </c>
+      <c r="G27" s="316">
+        <v>1.0246979551122099E-2</v>
+      </c>
+      <c r="H27" s="318">
+        <v>2.0563659268951599E-2</v>
+      </c>
+      <c r="I27" s="318">
+        <v>0.19738095238095199</v>
+      </c>
+      <c r="J27" s="316">
+        <v>6.3764662396113794E-2</v>
+      </c>
+      <c r="K27" s="316">
+        <v>2.8803688914402298E-4</v>
+      </c>
+      <c r="L27" s="316">
+        <v>0.33842253541432499</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="14">
+      <c r="A28" s="315" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="316">
+        <v>0</v>
+      </c>
+      <c r="C28" s="316">
+        <v>0</v>
+      </c>
+      <c r="D28" s="316">
+        <v>0.66109996541837801</v>
+      </c>
+      <c r="E28" s="316">
+        <v>0</v>
+      </c>
+      <c r="F28" s="316">
+        <v>0</v>
+      </c>
+      <c r="G28" s="316">
+        <v>0</v>
+      </c>
+      <c r="H28" s="316">
+        <v>1.7828976109525999E-2</v>
+      </c>
+      <c r="I28" s="316">
+        <v>0.26142857142857101</v>
+      </c>
+      <c r="J28" s="316">
+        <v>0.240072484689516</v>
+      </c>
+      <c r="K28" s="316">
+        <v>1.15214755657609E-2</v>
+      </c>
+      <c r="L28" s="316">
+        <v>0.69045041709366495</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="14">
+      <c r="A29" s="315" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="316">
+        <v>0</v>
+      </c>
+      <c r="C29" s="316">
+        <v>0</v>
+      </c>
+      <c r="D29" s="316">
+        <v>0.67524369596643696</v>
+      </c>
+      <c r="E29" s="316">
+        <v>0</v>
+      </c>
+      <c r="F29" s="316">
+        <v>0</v>
+      </c>
+      <c r="G29" s="316">
+        <v>0</v>
+      </c>
+      <c r="H29" s="316">
+        <v>0.50426672440086695</v>
+      </c>
+      <c r="I29" s="316">
+        <v>8.8809523809523797E-2</v>
+      </c>
+      <c r="J29" s="316">
+        <v>0.28973252130215699</v>
+      </c>
+      <c r="K29" s="316">
+        <v>4.6321568808706998E-2</v>
+      </c>
+      <c r="L29" s="316">
+        <v>1.2258319891760101</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="14">
+      <c r="A30" s="315" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="316">
+        <v>0</v>
+      </c>
+      <c r="C30" s="316">
+        <v>0</v>
+      </c>
+      <c r="D30" s="316">
+        <v>1.1829189077174</v>
+      </c>
+      <c r="E30" s="316">
+        <v>0</v>
+      </c>
+      <c r="F30" s="316">
+        <v>0</v>
+      </c>
+      <c r="G30" s="316">
+        <v>0</v>
+      </c>
+      <c r="H30" s="316">
+        <v>0.89142547202359701</v>
+      </c>
+      <c r="I30" s="316">
+        <v>0.108809523809523</v>
+      </c>
+      <c r="J30" s="316">
+        <v>0.26828173625646001</v>
+      </c>
+      <c r="K30" s="316">
+        <v>7.1695000225121402E-2</v>
+      </c>
+      <c r="L30" s="316">
+        <v>2.1460393799661199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="14">
+      <c r="A31" s="315" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="316">
+        <v>0</v>
+      </c>
+      <c r="C31" s="316">
+        <v>0</v>
+      </c>
+      <c r="D31" s="316">
+        <v>0.30077068878686702</v>
+      </c>
+      <c r="E31" s="316">
+        <v>0</v>
+      </c>
+      <c r="F31" s="316">
+        <v>0</v>
+      </c>
+      <c r="G31" s="316">
+        <v>0</v>
+      </c>
+      <c r="H31" s="316">
+        <v>0.22665514168512799</v>
+      </c>
+      <c r="I31" s="316">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="J31" s="316">
+        <v>0.37318489052103399</v>
+      </c>
+      <c r="K31" s="316">
+        <v>8.3006994416959506E-3</v>
+      </c>
+      <c r="L31" s="316">
+        <v>0.53572652991369196</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="14">
+      <c r="A32" s="315" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="316">
+        <v>0</v>
+      </c>
+      <c r="C32" s="316">
+        <v>0</v>
+      </c>
+      <c r="D32" s="316">
+        <v>4.4328329594462701E-2</v>
+      </c>
+      <c r="E32" s="316">
+        <v>0</v>
+      </c>
+      <c r="F32" s="316">
+        <v>0</v>
+      </c>
+      <c r="G32" s="316">
+        <v>0</v>
+      </c>
+      <c r="H32" s="316">
+        <v>1.8766852042601999E-2</v>
+      </c>
+      <c r="I32" s="316">
+        <v>0.12095238095238001</v>
+      </c>
+      <c r="J32" s="316">
+        <v>0.25065095402712001</v>
+      </c>
+      <c r="K32" s="316">
+        <v>3.3517019827668103E-2</v>
+      </c>
+      <c r="L32" s="316">
+        <v>9.66122014647329E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="14">
+      <c r="A33" s="315" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="316">
+        <v>0</v>
+      </c>
+      <c r="C33" s="316">
+        <v>7.1635728784688905E-4</v>
+      </c>
+      <c r="D33" s="316">
+        <v>1.7930560285400601E-2</v>
+      </c>
+      <c r="E33" s="316">
+        <v>0</v>
+      </c>
+      <c r="F33" s="316">
+        <v>0</v>
+      </c>
+      <c r="G33" s="316">
+        <v>0</v>
+      </c>
+      <c r="H33" s="316">
+        <v>1.2511234695068E-3</v>
+      </c>
+      <c r="I33" s="316">
+        <v>4.5238095238095202E-2</v>
+      </c>
+      <c r="J33" s="316">
+        <v>3.8787720904548503E-2</v>
+      </c>
+      <c r="K33" s="316">
+        <v>7.3318480873024098E-4</v>
+      </c>
+      <c r="L33" s="316">
+        <v>2.0631225851484501E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="14">
+      <c r="A34" s="315" t="s">
+        <v>21</v>
+      </c>
+      <c r="B34" s="316">
+        <v>0</v>
+      </c>
+      <c r="C34" s="316">
+        <v>0</v>
+      </c>
+      <c r="D34" s="316">
+        <v>2.0918986999634001E-2</v>
+      </c>
+      <c r="E34" s="316">
+        <v>0</v>
+      </c>
+      <c r="F34" s="316">
+        <v>0</v>
+      </c>
+      <c r="G34" s="316">
+        <v>0</v>
+      </c>
+      <c r="H34" s="316">
+        <v>0</v>
+      </c>
+      <c r="I34" s="316">
+        <v>6.6428571428571406E-2</v>
+      </c>
+      <c r="J34" s="316">
+        <v>8.9623142999146102E-2</v>
+      </c>
+      <c r="K34" s="316">
+        <v>1.9900730522677901E-3</v>
+      </c>
+      <c r="L34" s="316">
+        <v>2.2909060051901801E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="14">
+      <c r="A35" s="315" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="316">
+        <v>0</v>
+      </c>
+      <c r="C35" s="316">
+        <v>1.4327145756937701E-3</v>
+      </c>
+      <c r="D35" s="316">
+        <v>1.0459493499817001E-2</v>
+      </c>
+      <c r="E35" s="316">
+        <v>0</v>
+      </c>
+      <c r="F35" s="316">
+        <v>0</v>
+      </c>
+      <c r="G35" s="316">
+        <v>0</v>
+      </c>
+      <c r="H35" s="316">
+        <v>2.5022469390136E-3</v>
+      </c>
+      <c r="I35" s="316">
+        <v>3.0238095238095199E-2</v>
+      </c>
+      <c r="J35" s="316">
+        <v>3.82000281635705E-3</v>
+      </c>
+      <c r="K35" s="316">
+        <v>0</v>
+      </c>
+      <c r="L35" s="316">
+        <v>1.4394455014524399E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="14">
+      <c r="A36" s="315" t="s">
+        <v>23</v>
+      </c>
+      <c r="B36" s="316">
+        <v>4.5154969016487398E-2</v>
+      </c>
+      <c r="C36" s="316">
+        <v>7.5566954308935099E-4</v>
+      </c>
+      <c r="D36" s="316">
+        <v>6.6200940493026703E-2</v>
+      </c>
+      <c r="E36" s="316">
+        <v>1.28352971309176E-4</v>
+      </c>
+      <c r="F36" s="316">
+        <v>2.7116631353456599E-2</v>
+      </c>
+      <c r="G36" s="316">
+        <v>8.4179795511221903E-3</v>
+      </c>
+      <c r="H36" s="316">
+        <v>2.1116523223385801E-2</v>
+      </c>
+      <c r="I36" s="316">
+        <v>0</v>
+      </c>
+      <c r="J36" s="316">
+        <v>0</v>
+      </c>
+      <c r="K36" s="316">
+        <v>0</v>
+      </c>
+      <c r="L36" s="316">
+        <v>0.16889106615187699</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="14">
+      <c r="A37" s="315" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="316">
+        <v>0.100835955158491</v>
+      </c>
+      <c r="C37" s="316">
+        <v>0</v>
+      </c>
+      <c r="D37" s="316">
+        <v>0.23172878151125201</v>
+      </c>
+      <c r="E37" s="316">
+        <v>0</v>
+      </c>
+      <c r="F37" s="316">
+        <v>7.0446817916260895E-2</v>
+      </c>
+      <c r="G37" s="316">
+        <v>2.5014142144638402E-2</v>
+      </c>
+      <c r="H37" s="316">
+        <v>6.1412974418559897E-2</v>
+      </c>
+      <c r="I37" s="316">
+        <v>0</v>
+      </c>
+      <c r="J37" s="316">
+        <v>0</v>
+      </c>
+      <c r="K37" s="316">
+        <v>0</v>
+      </c>
+      <c r="L37" s="316">
+        <v>0.48943867114920298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="14">
+      <c r="A38" s="315" t="s">
+        <v>25</v>
+      </c>
+      <c r="B38" s="316">
+        <v>4.2580601581888797E-2</v>
+      </c>
+      <c r="C38" s="316">
+        <v>7.5534288416609298E-4</v>
+      </c>
+      <c r="D38" s="316">
+        <v>5.7244296405459402E-2</v>
+      </c>
+      <c r="E38" s="316">
+        <v>0</v>
+      </c>
+      <c r="F38" s="316">
+        <v>2.4640820447906501E-2</v>
+      </c>
+      <c r="G38" s="316">
+        <v>7.3625461346633397E-3</v>
+      </c>
+      <c r="H38" s="316">
+        <v>1.84689658001298E-2</v>
+      </c>
+      <c r="I38" s="316">
+        <v>0</v>
+      </c>
+      <c r="J38" s="316">
+        <v>0</v>
+      </c>
+      <c r="K38" s="316">
+        <v>0</v>
+      </c>
+      <c r="L38" s="316">
+        <v>0.15105257325421401</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="14">
+      <c r="A39" s="315" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" s="316">
+        <v>4.6252066014017901E-3</v>
+      </c>
+      <c r="C39" s="316">
+        <v>0</v>
+      </c>
+      <c r="D39" s="316">
+        <v>0</v>
+      </c>
+      <c r="E39" s="316">
+        <v>1.31617553460685E-3</v>
+      </c>
+      <c r="F39" s="316">
+        <v>0</v>
+      </c>
+      <c r="G39" s="316">
+        <v>1.7983511221945101E-3</v>
+      </c>
+      <c r="H39" s="316">
+        <v>2.6536278743300502E-3</v>
+      </c>
+      <c r="I39" s="316">
+        <v>0</v>
+      </c>
+      <c r="J39" s="316">
+        <v>0</v>
+      </c>
+      <c r="K39" s="316">
+        <v>0</v>
+      </c>
+      <c r="L39" s="316">
+        <v>1.03933611325332E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="14">
+      <c r="A40" s="315" t="s">
+        <v>27</v>
+      </c>
+      <c r="B40" s="316">
+        <v>4.8459471676373498E-4</v>
+      </c>
+      <c r="C40" s="316">
+        <v>0</v>
+      </c>
+      <c r="D40" s="316">
+        <v>4.4826400713501602E-4</v>
+      </c>
+      <c r="E40" s="316">
+        <v>0</v>
+      </c>
+      <c r="F40" s="316">
+        <v>0</v>
+      </c>
+      <c r="G40" s="316">
+        <v>1.4962593516209399E-4</v>
+      </c>
+      <c r="H40" s="316">
+        <v>2.5022469390135999E-4</v>
+      </c>
+      <c r="I40" s="316">
+        <v>0</v>
+      </c>
+      <c r="J40" s="316">
+        <v>0</v>
+      </c>
+      <c r="K40" s="316">
+        <v>0</v>
+      </c>
+      <c r="L40" s="316">
+        <v>1.3327093529621999E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="14">
+      <c r="A41" s="316" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="316">
+        <v>1.9221134453867601E-3</v>
+      </c>
+      <c r="C41" s="316">
+        <v>0</v>
+      </c>
+      <c r="D41" s="316">
+        <v>0</v>
+      </c>
+      <c r="E41" s="316">
+        <v>7.1763291251206499E-4</v>
+      </c>
+      <c r="F41" s="316">
+        <v>0</v>
+      </c>
+      <c r="G41" s="316">
+        <v>1.54821296758104E-3</v>
+      </c>
+      <c r="H41" s="316">
+        <v>7.76738736944317E-4</v>
+      </c>
+      <c r="I41" s="316">
+        <v>0</v>
+      </c>
+      <c r="J41" s="316">
+        <v>0</v>
+      </c>
+      <c r="K41" s="316">
+        <v>0</v>
+      </c>
+      <c r="L41" s="316">
+        <v>4.96469806242419E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="14">
       <c r="A42" s="206"/>
     </row>
-    <row r="43" spans="1:1" ht="14">
+    <row r="43" spans="1:12" ht="14">
       <c r="A43" s="206"/>
     </row>
-    <row r="44" spans="1:1" ht="14">
+    <row r="44" spans="1:12" ht="14">
       <c r="A44" s="206"/>
     </row>
-    <row r="45" spans="1:1" ht="14">
+    <row r="45" spans="1:12" ht="14">
       <c r="A45" s="206"/>
     </row>
-    <row r="46" spans="1:1" ht="14">
+    <row r="46" spans="1:12" ht="14">
       <c r="A46" s="206"/>
     </row>
-    <row r="47" spans="1:1" ht="14">
+    <row r="47" spans="1:12" ht="14">
       <c r="A47" s="206"/>
     </row>
-    <row r="48" spans="1:1" ht="14">
+    <row r="48" spans="1:12" ht="14">
       <c r="A48" s="206"/>
     </row>
     <row r="49" spans="1:1" ht="14">
@@ -43585,6 +45146,7 @@
       <c r="A959" s="206"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="C7:C10 D9:E9">
     <cfRule type="containsBlanks" dxfId="12" priority="11"/>
   </conditionalFormatting>
@@ -43608,9 +45170,6 @@
   </conditionalFormatting>
   <conditionalFormatting sqref="F10">
     <cfRule type="containsBlanks" dxfId="5" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H13">
-    <cfRule type="containsBlanks" dxfId="4" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -44508,28 +46067,28 @@
       <c r="D3" s="132"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="B4" s="290" t="s">
+      <c r="B4" s="289" t="s">
         <v>166</v>
       </c>
-      <c r="C4" s="290"/>
-      <c r="D4" s="290"/>
-      <c r="E4" s="290"/>
-      <c r="F4" s="290"/>
-      <c r="G4" s="290"/>
-      <c r="H4" s="290"/>
-      <c r="I4" s="290"/>
-      <c r="J4" s="290"/>
-      <c r="K4" s="290"/>
-      <c r="L4" s="290"/>
-      <c r="M4" s="290"/>
-      <c r="N4" s="290"/>
-      <c r="O4" s="290"/>
-      <c r="P4" s="291"/>
-      <c r="Q4" s="292" t="s">
+      <c r="C4" s="289"/>
+      <c r="D4" s="289"/>
+      <c r="E4" s="289"/>
+      <c r="F4" s="289"/>
+      <c r="G4" s="289"/>
+      <c r="H4" s="289"/>
+      <c r="I4" s="289"/>
+      <c r="J4" s="289"/>
+      <c r="K4" s="289"/>
+      <c r="L4" s="289"/>
+      <c r="M4" s="289"/>
+      <c r="N4" s="289"/>
+      <c r="O4" s="289"/>
+      <c r="P4" s="290"/>
+      <c r="Q4" s="291" t="s">
         <v>167</v>
       </c>
-      <c r="R4" s="293"/>
-      <c r="S4" s="293"/>
+      <c r="R4" s="292"/>
+      <c r="S4" s="292"/>
     </row>
     <row r="5" spans="1:19" s="133" customFormat="1" ht="46.5" customHeight="1">
       <c r="B5" s="133" t="s">
@@ -50541,16 +52100,16 @@
       </c>
     </row>
     <row r="35" spans="1:13">
-      <c r="A35" s="294" t="s">
+      <c r="A35" s="293" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="295"/>
-      <c r="C35" s="295"/>
-      <c r="D35" s="295"/>
-      <c r="E35" s="295"/>
-      <c r="F35" s="295"/>
-      <c r="G35" s="295"/>
-      <c r="H35" s="295"/>
+      <c r="B35" s="294"/>
+      <c r="C35" s="294"/>
+      <c r="D35" s="294"/>
+      <c r="E35" s="294"/>
+      <c r="F35" s="294"/>
+      <c r="G35" s="294"/>
+      <c r="H35" s="294"/>
       <c r="L35" t="s">
         <v>249</v>
       </c>
@@ -50559,14 +52118,14 @@
       </c>
     </row>
     <row r="36" spans="1:13">
-      <c r="A36" s="294"/>
-      <c r="B36" s="295"/>
-      <c r="C36" s="295"/>
-      <c r="D36" s="295"/>
-      <c r="E36" s="295"/>
-      <c r="F36" s="295"/>
-      <c r="G36" s="295"/>
-      <c r="H36" s="295"/>
+      <c r="A36" s="293"/>
+      <c r="B36" s="294"/>
+      <c r="C36" s="294"/>
+      <c r="D36" s="294"/>
+      <c r="E36" s="294"/>
+      <c r="F36" s="294"/>
+      <c r="G36" s="294"/>
+      <c r="H36" s="294"/>
       <c r="L36" t="s">
         <v>250</v>
       </c>
@@ -50654,26 +52213,26 @@
       </c>
     </row>
     <row r="43" spans="1:13">
-      <c r="A43" s="294" t="s">
+      <c r="A43" s="293" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="295"/>
-      <c r="C43" s="295"/>
-      <c r="D43" s="295"/>
-      <c r="E43" s="295"/>
-      <c r="F43" s="295"/>
-      <c r="G43" s="295"/>
-      <c r="H43" s="295"/>
+      <c r="B43" s="294"/>
+      <c r="C43" s="294"/>
+      <c r="D43" s="294"/>
+      <c r="E43" s="294"/>
+      <c r="F43" s="294"/>
+      <c r="G43" s="294"/>
+      <c r="H43" s="294"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="A44" s="294"/>
-      <c r="B44" s="295"/>
-      <c r="C44" s="295"/>
-      <c r="D44" s="295"/>
-      <c r="E44" s="295"/>
-      <c r="F44" s="295"/>
-      <c r="G44" s="295"/>
-      <c r="H44" s="295"/>
+      <c r="A44" s="293"/>
+      <c r="B44" s="294"/>
+      <c r="C44" s="294"/>
+      <c r="D44" s="294"/>
+      <c r="E44" s="294"/>
+      <c r="F44" s="294"/>
+      <c r="G44" s="294"/>
+      <c r="H44" s="294"/>
       <c r="L44" s="1" t="s">
         <v>101</v>
       </c>

</xml_diff>